<commit_message>
Build site at 2022-02-25 16:22:31 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -6403,10 +6403,10 @@
         <v>471</v>
       </c>
       <c r="C413" s="2" t="s">
-        <v>437</v>
+        <v>57</v>
       </c>
       <c r="D413" s="2" t="s">
-        <v>438</v>
+        <v>58</v>
       </c>
       <c r="E413" s="2"/>
     </row>
@@ -6814,10 +6814,10 @@
         <v>517</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>335</v>
+        <v>277</v>
       </c>
       <c r="D467" s="2" t="s">
-        <v>336</v>
+        <v>278</v>
       </c>
       <c r="E467" s="2"/>
     </row>

</xml_diff>

<commit_message>
Build site at 2022-03-11 16:24:32 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="961">
   <si>
     <t>Sigla</t>
   </si>
@@ -277,10 +277,10 @@
     <t xml:space="preserve"> Geometria Analítica</t>
   </si>
   <si>
-    <t>8884940</t>
-  </si>
-  <si>
-    <t>Paula Cristiane Pinto Mesquita Pardal</t>
+    <t>3682251</t>
+  </si>
+  <si>
+    <t>Gabrielle Weber Martins</t>
   </si>
   <si>
     <t>LOB1037</t>
@@ -1646,12 +1646,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Mecânica Clássica</t>
-  </si>
-  <si>
-    <t>3682251</t>
-  </si>
-  <si>
-    <t>Gabrielle Weber Martins</t>
   </si>
   <si>
     <t>5729033</t>
@@ -7054,10 +7048,10 @@
     </row>
     <row r="499" spans="1:5">
       <c r="C499" t="s">
-        <v>544</v>
+        <v>87</v>
       </c>
       <c r="D499" t="s">
-        <v>545</v>
+        <v>88</v>
       </c>
     </row>
     <row r="500" spans="1:5">
@@ -7070,18 +7064,18 @@
     </row>
     <row r="501" spans="1:5">
       <c r="C501" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D501" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="503" spans="1:5">
       <c r="A503" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B503" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C503" s="2" t="s">
         <v>335</v>
@@ -7093,10 +7087,10 @@
     </row>
     <row r="505" spans="1:5">
       <c r="A505" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B505" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C505" s="2" t="s">
         <v>275</v>
@@ -7124,10 +7118,10 @@
     </row>
     <row r="509" spans="1:5">
       <c r="A509" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B509" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C509" s="2" t="s">
         <v>335</v>
@@ -7147,85 +7141,85 @@
     </row>
     <row r="512" spans="1:5">
       <c r="A512" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B512" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C512" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="B512" s="2" t="s">
+      <c r="D512" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="C512" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="D512" s="2" t="s">
-        <v>557</v>
       </c>
       <c r="E512" s="2"/>
     </row>
     <row r="514" spans="1:5">
       <c r="A514" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B514" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C514" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="B514" s="2" t="s">
+      <c r="D514" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="C514" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="D514" s="2" t="s">
-        <v>561</v>
       </c>
       <c r="E514" s="2"/>
     </row>
     <row r="516" spans="1:5">
       <c r="A516" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C516" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="B516" s="2" t="s">
+      <c r="D516" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="C516" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="D516" s="2" t="s">
-        <v>565</v>
       </c>
       <c r="E516" s="2"/>
     </row>
     <row r="518" spans="1:5">
       <c r="A518" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B518" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C518" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="B518" s="2" t="s">
+      <c r="D518" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="C518" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="D518" s="2" t="s">
-        <v>569</v>
       </c>
       <c r="E518" s="2"/>
     </row>
     <row r="520" spans="1:5">
       <c r="A520" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B520" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C520" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="B520" s="2" t="s">
+      <c r="D520" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="C520" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="D520" s="2" t="s">
-        <v>573</v>
       </c>
       <c r="E520" s="2"/>
     </row>
     <row r="522" spans="1:5">
       <c r="A522" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C522" s="2" t="s">
         <v>29</v>
@@ -7237,85 +7231,85 @@
     </row>
     <row r="524" spans="1:5">
       <c r="A524" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B524" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="C524" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B524" s="2" t="s">
+      <c r="D524" s="2" t="s">
         <v>577</v>
-      </c>
-      <c r="C524" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="D524" s="2" t="s">
-        <v>579</v>
       </c>
       <c r="E524" s="2"/>
     </row>
     <row r="526" spans="1:5">
       <c r="A526" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B526" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C526" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="B526" s="2" t="s">
+      <c r="D526" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="C526" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="D526" s="2" t="s">
-        <v>583</v>
       </c>
       <c r="E526" s="2"/>
     </row>
     <row r="528" spans="1:5">
       <c r="A528" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C528" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D528" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E528" s="2"/>
     </row>
     <row r="530" spans="1:5">
       <c r="A530" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B530" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C530" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="B530" s="2" t="s">
+      <c r="D530" s="2" t="s">
         <v>587</v>
-      </c>
-      <c r="C530" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="D530" s="2" t="s">
-        <v>589</v>
       </c>
       <c r="E530" s="2"/>
     </row>
     <row r="532" spans="1:5">
       <c r="A532" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B532" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="C532" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="B532" s="2" t="s">
+      <c r="D532" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="C532" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D532" s="2" t="s">
-        <v>593</v>
       </c>
       <c r="E532" s="2"/>
     </row>
     <row r="534" spans="1:5">
       <c r="A534" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C534" s="2" t="s">
         <v>13</v>
@@ -7327,63 +7321,63 @@
     </row>
     <row r="536" spans="1:5">
       <c r="A536" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B536" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="C536" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="B536" s="2" t="s">
+      <c r="D536" s="2" t="s">
         <v>597</v>
-      </c>
-      <c r="C536" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="D536" s="2" t="s">
-        <v>599</v>
       </c>
       <c r="E536" s="2"/>
     </row>
     <row r="538" spans="1:5">
       <c r="A538" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B538" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C538" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="B538" s="2" t="s">
+      <c r="D538" s="2" t="s">
         <v>601</v>
-      </c>
-      <c r="C538" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="D538" s="2" t="s">
-        <v>603</v>
       </c>
       <c r="E538" s="2"/>
     </row>
     <row r="540" spans="1:5">
       <c r="A540" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B540" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="C540" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="B540" s="2" t="s">
+      <c r="D540" s="2" t="s">
         <v>605</v>
-      </c>
-      <c r="C540" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="D540" s="2" t="s">
-        <v>607</v>
       </c>
       <c r="E540" s="2"/>
     </row>
     <row r="541" spans="1:5">
       <c r="C541" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D541" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="543" spans="1:5">
       <c r="A543" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B543" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C543" s="2" t="s">
         <v>13</v>
@@ -7395,25 +7389,25 @@
     </row>
     <row r="545" spans="1:5">
       <c r="A545" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B545" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C545" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D545" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E545" s="2"/>
     </row>
     <row r="547" spans="1:5">
       <c r="A547" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B547" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C547" s="2" t="s">
         <v>111</v>
@@ -7425,10 +7419,10 @@
     </row>
     <row r="549" spans="1:5">
       <c r="A549" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B549" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C549" s="2" t="s">
         <v>111</v>
@@ -7440,7 +7434,7 @@
     </row>
     <row r="551" spans="1:5">
       <c r="A551" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B551" s="2" t="s">
         <v>354</v>
@@ -7455,10 +7449,10 @@
     </row>
     <row r="553" spans="1:5">
       <c r="A553" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B553" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C553" s="2" t="s">
         <v>7</v>
@@ -7470,491 +7464,491 @@
     </row>
     <row r="555" spans="1:5">
       <c r="A555" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B555" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C555" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="B555" s="2" t="s">
+      <c r="D555" s="2" t="s">
         <v>620</v>
-      </c>
-      <c r="C555" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="D555" s="2" t="s">
-        <v>622</v>
       </c>
       <c r="E555" s="2"/>
     </row>
     <row r="557" spans="1:5">
       <c r="A557" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="B557" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C557" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="B557" s="2" t="s">
+      <c r="D557" s="2" t="s">
         <v>624</v>
-      </c>
-      <c r="C557" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="D557" s="2" t="s">
-        <v>626</v>
       </c>
       <c r="E557" s="2"/>
     </row>
     <row r="559" spans="1:5">
       <c r="A559" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B559" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="C559" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="B559" s="2" t="s">
+      <c r="D559" s="2" t="s">
         <v>628</v>
-      </c>
-      <c r="C559" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="D559" s="2" t="s">
-        <v>630</v>
       </c>
       <c r="E559" s="2"/>
     </row>
     <row r="561" spans="1:5">
       <c r="A561" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B561" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="C561" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="B561" s="2" t="s">
+      <c r="D561" s="2" t="s">
         <v>632</v>
-      </c>
-      <c r="C561" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="D561" s="2" t="s">
-        <v>634</v>
       </c>
       <c r="E561" s="2"/>
     </row>
     <row r="563" spans="1:5">
       <c r="A563" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B563" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="C563" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="B563" s="2" t="s">
+      <c r="D563" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="C563" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="D563" s="2" t="s">
-        <v>638</v>
       </c>
       <c r="E563" s="2"/>
     </row>
     <row r="565" spans="1:5">
       <c r="A565" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B565" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="C565" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="B565" s="2" t="s">
+      <c r="D565" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="C565" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="D565" s="2" t="s">
-        <v>642</v>
       </c>
       <c r="E565" s="2"/>
     </row>
     <row r="567" spans="1:5">
       <c r="A567" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B567" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C567" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="B567" s="2" t="s">
+      <c r="D567" s="2" t="s">
         <v>644</v>
-      </c>
-      <c r="C567" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="D567" s="2" t="s">
-        <v>646</v>
       </c>
       <c r="E567" s="2"/>
     </row>
     <row r="569" spans="1:5">
       <c r="A569" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B569" s="2" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C569" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D569" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E569" s="2"/>
     </row>
     <row r="571" spans="1:5">
       <c r="A571" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B571" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="C571" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="B571" s="2" t="s">
+      <c r="D571" s="2" t="s">
         <v>650</v>
-      </c>
-      <c r="C571" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="D571" s="2" t="s">
-        <v>652</v>
       </c>
       <c r="E571" s="2"/>
     </row>
     <row r="573" spans="1:5">
       <c r="A573" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="B573" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="C573" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="B573" s="2" t="s">
+      <c r="D573" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="C573" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="D573" s="2" t="s">
-        <v>656</v>
       </c>
       <c r="E573" s="2"/>
     </row>
     <row r="574" spans="1:5">
       <c r="C574" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D574" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="576" spans="1:5">
       <c r="A576" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="B576" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="C576" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="B576" s="2" t="s">
+      <c r="D576" s="2" t="s">
         <v>658</v>
-      </c>
-      <c r="C576" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="D576" s="2" t="s">
-        <v>660</v>
       </c>
       <c r="E576" s="2"/>
     </row>
     <row r="578" spans="1:5">
       <c r="A578" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C578" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D578" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E578" s="2"/>
     </row>
     <row r="580" spans="1:5">
       <c r="A580" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C580" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D580" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E580" s="2"/>
     </row>
     <row r="582" spans="1:5">
       <c r="A582" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C582" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D582" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E582" s="2"/>
     </row>
     <row r="584" spans="1:5">
       <c r="A584" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C584" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D584" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E584" s="2"/>
     </row>
     <row r="586" spans="1:5">
       <c r="A586" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C586" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D586" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E586" s="2"/>
     </row>
     <row r="588" spans="1:5">
       <c r="A588" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C588" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D588" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E588" s="2"/>
     </row>
     <row r="590" spans="1:5">
       <c r="A590" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C590" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D590" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E590" s="2"/>
     </row>
     <row r="592" spans="1:5">
       <c r="A592" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C592" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D592" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E592" s="2"/>
     </row>
     <row r="594" spans="1:5">
       <c r="A594" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B594" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C594" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D594" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E594" s="2"/>
     </row>
     <row r="596" spans="1:5">
       <c r="A596" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="B596" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C596" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="B596" s="2" t="s">
+      <c r="D596" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="C596" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="D596" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="E596" s="2"/>
     </row>
     <row r="598" spans="1:5">
       <c r="A598" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="B598" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C598" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="B598" s="2" t="s">
+      <c r="D598" s="2" t="s">
         <v>684</v>
-      </c>
-      <c r="C598" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="D598" s="2" t="s">
-        <v>686</v>
       </c>
       <c r="E598" s="2"/>
     </row>
     <row r="600" spans="1:5">
       <c r="A600" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B600" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C600" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D600" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E600" s="2"/>
     </row>
     <row r="602" spans="1:5">
       <c r="A602" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B602" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="C602" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="B602" s="2" t="s">
+      <c r="D602" s="2" t="s">
         <v>690</v>
-      </c>
-      <c r="C602" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="D602" s="2" t="s">
-        <v>692</v>
       </c>
       <c r="E602" s="2"/>
     </row>
     <row r="604" spans="1:5">
       <c r="A604" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="B604" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="C604" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="B604" s="2" t="s">
+      <c r="D604" s="2" t="s">
         <v>694</v>
-      </c>
-      <c r="C604" s="2" t="s">
-        <v>695</v>
-      </c>
-      <c r="D604" s="2" t="s">
-        <v>696</v>
       </c>
       <c r="E604" s="2"/>
     </row>
     <row r="606" spans="1:5">
       <c r="A606" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C606" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D606" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="E606" s="2"/>
     </row>
     <row r="608" spans="1:5">
       <c r="A608" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C608" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D608" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E608" s="2"/>
     </row>
     <row r="610" spans="1:5">
       <c r="A610" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C610" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D610" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E610" s="2"/>
     </row>
     <row r="612" spans="1:5">
       <c r="A612" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B612" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C612" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D612" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E612" s="2"/>
     </row>
     <row r="613" spans="1:5">
       <c r="C613" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D613" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="615" spans="1:5">
       <c r="A615" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B615" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C615" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D615" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E615" s="2"/>
     </row>
     <row r="617" spans="1:5">
       <c r="A617" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B617" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C617" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D617" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E617" s="2"/>
     </row>
     <row r="619" spans="1:5">
       <c r="A619" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B619" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C619" s="2" t="s">
         <v>13</v>
@@ -7966,117 +7960,117 @@
     </row>
     <row r="620" spans="1:5">
       <c r="C620" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D620" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="621" spans="1:5">
       <c r="C621" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D621" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="622" spans="1:5">
       <c r="C622" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D622" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="624" spans="1:5">
       <c r="A624" s="2" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C624" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D624" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E624" s="2"/>
     </row>
     <row r="626" spans="1:5">
       <c r="A626" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C626" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D626" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E626" s="2"/>
     </row>
     <row r="628" spans="1:5">
       <c r="A628" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C628" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D628" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E628" s="2"/>
     </row>
     <row r="630" spans="1:5">
       <c r="A630" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="B630" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="C630" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="B630" s="2" t="s">
+      <c r="D630" s="2" t="s">
         <v>718</v>
-      </c>
-      <c r="C630" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="D630" s="2" t="s">
-        <v>720</v>
       </c>
       <c r="E630" s="2"/>
     </row>
     <row r="631" spans="1:5">
       <c r="C631" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D631" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="633" spans="1:5">
       <c r="A633" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B633" s="2" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C633" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D633" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E633" s="2"/>
     </row>
     <row r="635" spans="1:5">
       <c r="A635" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B635" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C635" s="2" t="s">
         <v>13</v>
@@ -8088,214 +8082,214 @@
     </row>
     <row r="636" spans="1:5">
       <c r="C636" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D636" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="638" spans="1:5">
       <c r="A638" s="2" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C638" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D638" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E638" s="2"/>
     </row>
     <row r="639" spans="1:5">
       <c r="C639" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D639" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="641" spans="1:5">
       <c r="A641" s="2" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B641" s="2" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C641" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D641" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E641" s="2"/>
     </row>
     <row r="643" spans="1:5">
       <c r="A643" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C643" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D643" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E643" s="2"/>
     </row>
     <row r="644" spans="1:5">
       <c r="C644" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D644" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="646" spans="1:5">
       <c r="A646" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B646" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C646" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="B646" s="2" t="s">
+      <c r="D646" s="2" t="s">
         <v>736</v>
-      </c>
-      <c r="C646" s="2" t="s">
-        <v>737</v>
-      </c>
-      <c r="D646" s="2" t="s">
-        <v>738</v>
       </c>
       <c r="E646" s="2"/>
     </row>
     <row r="648" spans="1:5">
       <c r="A648" s="2" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C648" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D648" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E648" s="2"/>
     </row>
     <row r="650" spans="1:5">
       <c r="A650" s="2" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C650" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D650" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E650" s="2"/>
     </row>
     <row r="652" spans="1:5">
       <c r="A652" s="2" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C652" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D652" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E652" s="2"/>
     </row>
     <row r="654" spans="1:5">
       <c r="A654" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="B654" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C654" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="B654" s="2" t="s">
+      <c r="D654" s="2" t="s">
         <v>746</v>
-      </c>
-      <c r="C654" s="2" t="s">
-        <v>747</v>
-      </c>
-      <c r="D654" s="2" t="s">
-        <v>748</v>
       </c>
       <c r="E654" s="2"/>
     </row>
     <row r="656" spans="1:5">
       <c r="A656" s="2" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C656" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D656" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E656" s="2"/>
     </row>
     <row r="658" spans="1:5">
       <c r="A658" s="2" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C658" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D658" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E658" s="2"/>
     </row>
     <row r="660" spans="1:5">
       <c r="A660" s="2" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C660" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D660" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E660" s="2"/>
     </row>
     <row r="662" spans="1:5">
       <c r="A662" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="B662" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="C662" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="B662" s="2" t="s">
+      <c r="D662" s="2" t="s">
         <v>756</v>
-      </c>
-      <c r="C662" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="D662" s="2" t="s">
-        <v>758</v>
       </c>
       <c r="E662" s="2"/>
     </row>
     <row r="664" spans="1:5">
       <c r="A664" s="2" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C664" s="2" t="s">
         <v>7</v>
@@ -8307,70 +8301,70 @@
     </row>
     <row r="666" spans="1:5">
       <c r="A666" s="2" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C666" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D666" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E666" s="2"/>
     </row>
     <row r="668" spans="1:5">
       <c r="A668" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C668" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D668" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E668" s="2"/>
     </row>
     <row r="670" spans="1:5">
       <c r="A670" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C670" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D670" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E670" s="2"/>
     </row>
     <row r="672" spans="1:5">
       <c r="A672" s="2" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C672" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D672" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E672" s="2"/>
     </row>
     <row r="674" spans="1:5">
       <c r="A674" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C674" s="2" t="s">
         <v>13</v>
@@ -8382,10 +8376,10 @@
     </row>
     <row r="676" spans="1:5">
       <c r="A676" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C676" s="2" t="s">
         <v>7</v>
@@ -8397,10 +8391,10 @@
     </row>
     <row r="678" spans="1:5">
       <c r="A678" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C678" s="2" t="s">
         <v>111</v>
@@ -8412,25 +8406,25 @@
     </row>
     <row r="680" spans="1:5">
       <c r="A680" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C680" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D680" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E680" s="2"/>
     </row>
     <row r="682" spans="1:5">
       <c r="A682" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C682" s="2" t="s">
         <v>29</v>
@@ -8442,10 +8436,10 @@
     </row>
     <row r="684" spans="1:5">
       <c r="A684" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C684" s="2" t="s">
         <v>7</v>
@@ -8457,10 +8451,10 @@
     </row>
     <row r="686" spans="1:5">
       <c r="A686" s="2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C686" s="2" t="s">
         <v>7</v>
@@ -8472,10 +8466,10 @@
     </row>
     <row r="688" spans="1:5">
       <c r="A688" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C688" s="2" t="s">
         <v>7</v>
@@ -8487,10 +8481,10 @@
     </row>
     <row r="690" spans="1:5">
       <c r="A690" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C690" s="2" t="s">
         <v>7</v>
@@ -8502,10 +8496,10 @@
     </row>
     <row r="692" spans="1:5">
       <c r="A692" s="2" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C692" s="2" t="s">
         <v>7</v>
@@ -8517,16 +8511,16 @@
     </row>
     <row r="694" spans="1:5">
       <c r="A694" s="2" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C694" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D694" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E694" s="2"/>
     </row>
@@ -8540,40 +8534,40 @@
     </row>
     <row r="697" spans="1:5">
       <c r="A697" s="2" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B697" s="2" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C697" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D697" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E697" s="2"/>
     </row>
     <row r="699" spans="1:5">
       <c r="A699" s="2" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B699" s="2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C699" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D699" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E699" s="2"/>
     </row>
     <row r="701" spans="1:5">
       <c r="A701" s="2" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B701" s="2" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C701" s="2" t="s">
         <v>125</v>
@@ -8585,40 +8579,40 @@
     </row>
     <row r="703" spans="1:5">
       <c r="A703" s="2" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B703" s="2" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C703" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D703" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E703" s="2"/>
     </row>
     <row r="705" spans="1:5">
       <c r="A705" s="2" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B705" s="2" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C705" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D705" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E705" s="2"/>
     </row>
     <row r="707" spans="1:5">
       <c r="A707" s="2" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B707" s="2" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C707" s="2" t="s">
         <v>125</v>
@@ -8630,25 +8624,25 @@
     </row>
     <row r="709" spans="1:5">
       <c r="A709" s="2" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B709" s="2" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C709" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D709" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E709" s="2"/>
     </row>
     <row r="711" spans="1:5">
       <c r="A711" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B711" s="2" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="C711" s="2" t="s">
         <v>7</v>
@@ -8660,10 +8654,10 @@
     </row>
     <row r="713" spans="1:5">
       <c r="A713" s="2" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B713" s="2" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C713" s="2" t="s">
         <v>7</v>
@@ -8675,10 +8669,10 @@
     </row>
     <row r="715" spans="1:5">
       <c r="A715" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B715" s="2" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="C715" s="2" t="s">
         <v>13</v>
@@ -8690,40 +8684,40 @@
     </row>
     <row r="717" spans="1:5">
       <c r="A717" s="2" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B717" s="2" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C717" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D717" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E717" s="2"/>
     </row>
     <row r="719" spans="1:5">
       <c r="A719" s="2" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B719" s="2" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C719" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D719" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E719" s="2"/>
     </row>
     <row r="721" spans="1:5">
       <c r="A721" s="2" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B721" s="2" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C721" s="2" t="s">
         <v>7</v>
@@ -8735,70 +8729,70 @@
     </row>
     <row r="723" spans="1:5">
       <c r="A723" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B723" s="2" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C723" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D723" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E723" s="2"/>
     </row>
     <row r="725" spans="1:5">
       <c r="A725" s="2" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B725" s="2" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C725" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D725" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E725" s="2"/>
     </row>
     <row r="727" spans="1:5">
       <c r="A727" s="2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B727" s="2" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C727" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D727" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E727" s="2"/>
     </row>
     <row r="729" spans="1:5">
       <c r="A729" s="2" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B729" s="2" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C729" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D729" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E729" s="2"/>
     </row>
     <row r="731" spans="1:5">
       <c r="A731" s="2" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B731" s="2" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C731" s="2" t="s">
         <v>7</v>
@@ -8810,40 +8804,40 @@
     </row>
     <row r="733" spans="1:5">
       <c r="A733" s="2" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B733" s="2" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C733" s="2" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D733" s="2" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E733" s="2"/>
     </row>
     <row r="735" spans="1:5">
       <c r="A735" s="2" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B735" s="2" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C735" s="2" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D735" s="2" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E735" s="2"/>
     </row>
     <row r="737" spans="1:5">
       <c r="A737" s="2" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B737" s="2" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C737" s="2" t="s">
         <v>125</v>
@@ -8855,40 +8849,40 @@
     </row>
     <row r="739" spans="1:5">
       <c r="A739" s="2" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B739" s="2" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C739" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D739" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E739" s="2"/>
     </row>
     <row r="741" spans="1:5">
       <c r="A741" s="2" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B741" s="2" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C741" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D741" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E741" s="2"/>
     </row>
     <row r="743" spans="1:5">
       <c r="A743" s="2" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B743" s="2" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C743" s="2" t="s">
         <v>7</v>
@@ -8900,184 +8894,184 @@
     </row>
     <row r="744" spans="1:5">
       <c r="C744" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D744" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="746" spans="1:5">
       <c r="A746" s="2" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="C746" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D746" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E746" s="2"/>
     </row>
     <row r="748" spans="1:5">
       <c r="A748" s="2" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="C748" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D748" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E748" s="2"/>
     </row>
     <row r="750" spans="1:5">
       <c r="A750" s="2" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B750" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C750" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D750" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E750" s="2"/>
     </row>
     <row r="752" spans="1:5">
       <c r="A752" s="2" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B752" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C752" s="2" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D752" s="2" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E752" s="2"/>
     </row>
     <row r="754" spans="1:5">
       <c r="A754" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B754" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="C754" s="2" t="s">
         <v>845</v>
       </c>
-      <c r="B754" s="2" t="s">
+      <c r="D754" s="2" t="s">
         <v>846</v>
-      </c>
-      <c r="C754" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="D754" s="2" t="s">
-        <v>848</v>
       </c>
       <c r="E754" s="2"/>
     </row>
     <row r="755" spans="1:5">
       <c r="C755" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D755" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="757" spans="1:5">
       <c r="A757" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B757" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="C757" s="2" t="s">
         <v>851</v>
       </c>
-      <c r="B757" s="2" t="s">
+      <c r="D757" s="2" t="s">
         <v>852</v>
-      </c>
-      <c r="C757" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="D757" s="2" t="s">
-        <v>854</v>
       </c>
       <c r="E757" s="2"/>
     </row>
     <row r="758" spans="1:5">
       <c r="C758" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D758" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="760" spans="1:5">
       <c r="A760" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B760" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C760" s="2" t="s">
         <v>857</v>
       </c>
-      <c r="B760" s="2" t="s">
+      <c r="D760" s="2" t="s">
         <v>858</v>
-      </c>
-      <c r="C760" s="2" t="s">
-        <v>859</v>
-      </c>
-      <c r="D760" s="2" t="s">
-        <v>860</v>
       </c>
       <c r="E760" s="2"/>
     </row>
     <row r="762" spans="1:5">
       <c r="A762" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B762" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="C762" s="2" t="s">
         <v>861</v>
       </c>
-      <c r="B762" s="2" t="s">
+      <c r="D762" s="2" t="s">
         <v>862</v>
-      </c>
-      <c r="C762" s="2" t="s">
-        <v>863</v>
-      </c>
-      <c r="D762" s="2" t="s">
-        <v>864</v>
       </c>
       <c r="E762" s="2"/>
     </row>
     <row r="764" spans="1:5">
       <c r="A764" s="2" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B764" s="2" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C764" s="2" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D764" s="2" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="E764" s="2"/>
     </row>
     <row r="766" spans="1:5">
       <c r="A766" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B766" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C766" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="B766" s="2" t="s">
+      <c r="D766" s="2" t="s">
         <v>868</v>
-      </c>
-      <c r="C766" s="2" t="s">
-        <v>869</v>
-      </c>
-      <c r="D766" s="2" t="s">
-        <v>870</v>
       </c>
       <c r="E766" s="2"/>
     </row>
     <row r="768" spans="1:5">
       <c r="A768" s="2" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C768" s="2" t="s">
         <v>241</v>
@@ -9089,145 +9083,145 @@
     </row>
     <row r="770" spans="1:5">
       <c r="A770" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B770" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="C770" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="B770" s="2" t="s">
+      <c r="D770" s="2" t="s">
         <v>874</v>
-      </c>
-      <c r="C770" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="D770" s="2" t="s">
-        <v>876</v>
       </c>
       <c r="E770" s="2"/>
     </row>
     <row r="772" spans="1:5">
       <c r="A772" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="B772" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="C772" s="2" t="s">
         <v>877</v>
       </c>
-      <c r="B772" s="2" t="s">
+      <c r="D772" s="2" t="s">
         <v>878</v>
-      </c>
-      <c r="C772" s="2" t="s">
-        <v>879</v>
-      </c>
-      <c r="D772" s="2" t="s">
-        <v>880</v>
       </c>
       <c r="E772" s="2"/>
     </row>
     <row r="774" spans="1:5">
       <c r="A774" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B774" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="C774" s="2" t="s">
         <v>881</v>
       </c>
-      <c r="B774" s="2" t="s">
+      <c r="D774" s="2" t="s">
         <v>882</v>
-      </c>
-      <c r="C774" s="2" t="s">
-        <v>883</v>
-      </c>
-      <c r="D774" s="2" t="s">
-        <v>884</v>
       </c>
       <c r="E774" s="2"/>
     </row>
     <row r="776" spans="1:5">
       <c r="A776" s="2" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C776" s="2" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D776" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E776" s="2"/>
     </row>
     <row r="778" spans="1:5">
       <c r="A778" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="B778" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="C778" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="B778" s="2" t="s">
+      <c r="D778" s="2" t="s">
         <v>888</v>
-      </c>
-      <c r="C778" s="2" t="s">
-        <v>889</v>
-      </c>
-      <c r="D778" s="2" t="s">
-        <v>890</v>
       </c>
       <c r="E778" s="2"/>
     </row>
     <row r="780" spans="1:5">
       <c r="A780" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B780" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="C780" s="2" t="s">
         <v>891</v>
       </c>
-      <c r="B780" s="2" t="s">
+      <c r="D780" s="2" t="s">
         <v>892</v>
-      </c>
-      <c r="C780" s="2" t="s">
-        <v>893</v>
-      </c>
-      <c r="D780" s="2" t="s">
-        <v>894</v>
       </c>
       <c r="E780" s="2"/>
     </row>
     <row r="782" spans="1:5">
       <c r="A782" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="B782" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="C782" s="2" t="s">
         <v>895</v>
       </c>
-      <c r="B782" s="2" t="s">
+      <c r="D782" s="2" t="s">
         <v>896</v>
-      </c>
-      <c r="C782" s="2" t="s">
-        <v>897</v>
-      </c>
-      <c r="D782" s="2" t="s">
-        <v>898</v>
       </c>
       <c r="E782" s="2"/>
     </row>
     <row r="784" spans="1:5">
       <c r="A784" s="2" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C784" s="2" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="D784" s="2" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E784" s="2"/>
     </row>
     <row r="786" spans="1:5">
       <c r="A786" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="B786" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="C786" s="2" t="s">
         <v>901</v>
       </c>
-      <c r="B786" s="2" t="s">
+      <c r="D786" s="2" t="s">
         <v>902</v>
-      </c>
-      <c r="C786" s="2" t="s">
-        <v>903</v>
-      </c>
-      <c r="D786" s="2" t="s">
-        <v>904</v>
       </c>
       <c r="E786" s="2"/>
     </row>
     <row r="788" spans="1:5">
       <c r="A788" s="2" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C788" s="2" t="s">
         <v>241</v>
@@ -9239,433 +9233,433 @@
     </row>
     <row r="790" spans="1:5">
       <c r="A790" s="2" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C790" s="2" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D790" s="2" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E790" s="2"/>
     </row>
     <row r="792" spans="1:5">
       <c r="A792" s="2" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C792" s="2" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D792" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E792" s="2"/>
     </row>
     <row r="793" spans="1:5">
       <c r="C793" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D793" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="795" spans="1:5">
       <c r="A795" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="B795" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="C795" s="2" t="s">
         <v>913</v>
       </c>
-      <c r="B795" s="2" t="s">
+      <c r="D795" s="2" t="s">
         <v>914</v>
-      </c>
-      <c r="C795" s="2" t="s">
-        <v>915</v>
-      </c>
-      <c r="D795" s="2" t="s">
-        <v>916</v>
       </c>
       <c r="E795" s="2"/>
     </row>
     <row r="797" spans="1:5">
       <c r="A797" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B797" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="C797" s="2" t="s">
         <v>917</v>
       </c>
-      <c r="B797" s="2" t="s">
+      <c r="D797" s="2" t="s">
         <v>918</v>
-      </c>
-      <c r="C797" s="2" t="s">
-        <v>919</v>
-      </c>
-      <c r="D797" s="2" t="s">
-        <v>920</v>
       </c>
       <c r="E797" s="2"/>
     </row>
     <row r="799" spans="1:5">
       <c r="A799" s="2" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C799" s="2" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D799" s="2" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E799" s="2"/>
     </row>
     <row r="801" spans="1:5">
       <c r="A801" s="2" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C801" s="2" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D801" s="2" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E801" s="2"/>
     </row>
     <row r="802" spans="1:5">
       <c r="C802" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D802" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="804" spans="1:5">
       <c r="A804" s="2" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C804" s="2" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D804" s="2" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E804" s="2"/>
     </row>
     <row r="806" spans="1:5">
       <c r="A806" s="2" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C806" s="2" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D806" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E806" s="2"/>
     </row>
     <row r="807" spans="1:5">
       <c r="C807" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D807" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="809" spans="1:5">
       <c r="A809" s="2" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B809" s="2" t="s">
         <v>354</v>
       </c>
       <c r="C809" s="2" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D809" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E809" s="2"/>
     </row>
     <row r="811" spans="1:5">
       <c r="A811" s="2" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="C811" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D811" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E811" s="2"/>
     </row>
     <row r="813" spans="1:5">
       <c r="A813" s="2" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C813" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D813" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E813" s="2"/>
     </row>
     <row r="815" spans="1:5">
       <c r="A815" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C815" s="2" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D815" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E815" s="2"/>
     </row>
     <row r="817" spans="1:5">
       <c r="A817" s="2" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="C817" s="2" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D817" s="2" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E817" s="2"/>
     </row>
     <row r="819" spans="1:5">
       <c r="A819" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="B819" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="C819" s="2" t="s">
         <v>940</v>
       </c>
-      <c r="B819" s="2" t="s">
+      <c r="D819" s="2" t="s">
         <v>941</v>
-      </c>
-      <c r="C819" s="2" t="s">
-        <v>942</v>
-      </c>
-      <c r="D819" s="2" t="s">
-        <v>943</v>
       </c>
       <c r="E819" s="2"/>
     </row>
     <row r="820" spans="1:5">
       <c r="C820" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D820" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="822" spans="1:5">
       <c r="A822" s="2" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="C822" s="2" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D822" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E822" s="2"/>
     </row>
     <row r="824" spans="1:5">
       <c r="A824" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B824" s="2" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C824" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D824" s="2" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E824" s="2"/>
     </row>
     <row r="826" spans="1:5">
       <c r="A826" s="2" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B826" s="2" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="C826" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="D826" s="2" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E826" s="2"/>
     </row>
     <row r="827" spans="1:5">
       <c r="C827" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D827" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="829" spans="1:5">
       <c r="A829" s="2" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C829" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D829" s="2" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E829" s="2"/>
     </row>
     <row r="831" spans="1:5">
       <c r="A831" s="2" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="C831" s="2" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D831" s="2" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E831" s="2"/>
     </row>
     <row r="833" spans="1:5">
       <c r="A833" s="2" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C833" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D833" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E833" s="2"/>
     </row>
     <row r="834" spans="1:5">
       <c r="C834" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D834" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="836" spans="1:5">
       <c r="A836" s="2" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C836" s="2" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D836" s="2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E836" s="2"/>
     </row>
     <row r="837" spans="1:5">
       <c r="C837" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D837" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="839" spans="1:5">
       <c r="A839" s="2" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B839" s="2" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C839" s="2" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D839" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E839" s="2"/>
     </row>
     <row r="840" spans="1:5">
       <c r="C840" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D840" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="842" spans="1:5">
       <c r="A842" s="2" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C842" s="2" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D842" s="2" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E842" s="2"/>
     </row>
     <row r="843" spans="1:5">
       <c r="C843" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D843" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="845" spans="1:5">
       <c r="A845" s="2" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C845" s="2" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D845" s="2" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="E845" s="2"/>
     </row>

</xml_diff>

<commit_message>
Build site at 2022-10-03 16:06:37 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="703">
   <si>
     <t>Sigla</t>
   </si>
@@ -931,22 +931,22 @@
     <t xml:space="preserve"> Tratamentos de Minérios e Hidrometalurgia</t>
   </si>
   <si>
-    <t>LOM3201</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Biofísica Molecular</t>
-  </si>
-  <si>
-    <t>LOM3202</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Circuitos Elétricos</t>
-  </si>
-  <si>
-    <t>LOM3203</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Controle e Automação</t>
+    <t>LOM3114</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estatística Aplicada à Engenharia</t>
+  </si>
+  <si>
+    <t>LOM3115</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aplicações Tecnológicas Avançadas de Materiais Poliméricos</t>
+  </si>
+  <si>
+    <t>LOM3116</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Análise de Falhas de Materiais e Componentes</t>
   </si>
   <si>
     <t>LOM3204</t>
@@ -961,18 +961,6 @@
     <t xml:space="preserve"> Eletromagnetismo</t>
   </si>
   <si>
-    <t>LOM3206</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eletrônica</t>
-  </si>
-  <si>
-    <t>LOM3207</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eletrônica de Potência</t>
-  </si>
-  <si>
     <t>LOM3208</t>
   </si>
   <si>
@@ -982,12 +970,6 @@
     <t>LOM3210</t>
   </si>
   <si>
-    <t>LOM3211</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Estruturas e Propriedades de Materiais</t>
-  </si>
-  <si>
     <t>LOM3212</t>
   </si>
   <si>
@@ -1000,12 +982,6 @@
     <t xml:space="preserve"> Fenômenos de Transporte B</t>
   </si>
   <si>
-    <t>LOM3214</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Física de Superfícies</t>
-  </si>
-  <si>
     <t>LOM3215</t>
   </si>
   <si>
@@ -1036,36 +1012,12 @@
     <t xml:space="preserve"> Introdução à Spintrônica</t>
   </si>
   <si>
-    <t>LOM3221</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Laboratório de Eletrônica</t>
-  </si>
-  <si>
-    <t>LOM3222</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Materiais e Dispositivos Dielétricos e Piezelétricos</t>
-  </si>
-  <si>
     <t>LOM3223</t>
   </si>
   <si>
     <t xml:space="preserve"> Materiais e Dispositivos Magnéticos e Supercondutores</t>
   </si>
   <si>
-    <t>LOM3224</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Materiais e Dispositivos Ópticos e Fotônicos</t>
-  </si>
-  <si>
-    <t>LOM3225</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Materiais e Dispositivos Semicondutores</t>
-  </si>
-  <si>
     <t>LOM3226</t>
   </si>
   <si>
@@ -1102,12 +1054,6 @@
     <t xml:space="preserve"> Métodos Experimentais da Física III</t>
   </si>
   <si>
-    <t>LOM3231</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Métodos Experimentais da Física IV</t>
-  </si>
-  <si>
     <t>LOM3232</t>
   </si>
   <si>
@@ -1126,12 +1072,6 @@
     <t xml:space="preserve"> Óptica Física</t>
   </si>
   <si>
-    <t>LOM3235</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Processamento de Materiais</t>
-  </si>
-  <si>
     <t>LOM3236</t>
   </si>
   <si>
@@ -1141,13 +1081,7 @@
     <t>LOM3238</t>
   </si>
   <si>
-    <t xml:space="preserve"> Projeto Integrado I</t>
-  </si>
-  <si>
-    <t>LOM3239</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Projeto Integrado II</t>
+    <t xml:space="preserve"> Projeto Integrado</t>
   </si>
   <si>
     <t>LOM3240</t>
@@ -1174,30 +1108,12 @@
     <t xml:space="preserve"> Seminários em Engenharia Física</t>
   </si>
   <si>
-    <t>LOM3244</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sensores e Transdutores</t>
-  </si>
-  <si>
-    <t>LOM3245</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Técnicas Avançadas de Caracterização de Materiais</t>
-  </si>
-  <si>
     <t>LOM3246</t>
   </si>
   <si>
     <t xml:space="preserve"> Técnicas de Caracterização de Materiais</t>
   </si>
   <si>
-    <t>LOM3247</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Técnicas de Análises Espectroscópicas</t>
-  </si>
-  <si>
     <t>LOM3248</t>
   </si>
   <si>
@@ -1213,37 +1129,16 @@
     <t>LOM3250</t>
   </si>
   <si>
-    <t xml:space="preserve"> Trabalho de Graduação</t>
-  </si>
-  <si>
-    <t>LOM3251</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vibração e Acústica</t>
-  </si>
-  <si>
     <t>LOM3253</t>
   </si>
   <si>
     <t xml:space="preserve"> Física Matemática</t>
   </si>
   <si>
-    <t>LOM3254</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Laboratório de Circuitos Elétricos</t>
-  </si>
-  <si>
-    <t>LOM3255</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Introdução a Projetos de Engenharia</t>
-  </si>
-  <si>
     <t>LOM3256</t>
   </si>
   <si>
-    <t xml:space="preserve"> Tópicos em Cálculo de Estrutura Eletrônica dos Materiais</t>
+    <t xml:space="preserve"> Tópicos em Cálculo de Estrutura Eletrônica</t>
   </si>
   <si>
     <t>LOM3257</t>
@@ -1270,6 +1165,51 @@
     <t xml:space="preserve"> Computação Científica em Python</t>
   </si>
   <si>
+    <t>LOM3261</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Métodos Numéricos e Aplicações</t>
+  </si>
+  <si>
+    <t>LOM3262</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Circuitos Elétricos - teoria e prática</t>
+  </si>
+  <si>
+    <t>LOM3263</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eletrônica Fundamental e Aplicada</t>
+  </si>
+  <si>
+    <t>LOM3264</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fundamentos de Controle</t>
+  </si>
+  <si>
+    <t>LOM3265</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Automação</t>
+  </si>
+  <si>
+    <t>LOM3266</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fotônica Integrada</t>
+  </si>
+  <si>
+    <t>LOM3267</t>
+  </si>
+  <si>
+    <t>LOM3268</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Projeto Computacional</t>
+  </si>
+  <si>
     <t>LOQ4001</t>
   </si>
   <si>
@@ -1334,12 +1274,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Processos Químicos Industriais II</t>
-  </si>
-  <si>
-    <t>LOQ4031</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Química Geral I</t>
   </si>
   <si>
     <t>LOQ4037</t>
@@ -2539,7 +2473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E724"/>
+  <dimension ref="A1:E704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3843,23 +3777,23 @@
         <v>317</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>318</v>
+        <v>238</v>
       </c>
     </row>
     <row r="316" spans="1:5">
       <c r="A316" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B316" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="318" spans="1:5">
       <c r="A318" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B318" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="320" spans="1:5">
@@ -3870,7 +3804,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:5">
       <c r="A322" s="2" t="s">
         <v>324</v>
       </c>
@@ -3878,7 +3812,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:5">
       <c r="A324" s="2" t="s">
         <v>326</v>
       </c>
@@ -3886,7 +3820,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:5">
       <c r="A326" s="2" t="s">
         <v>328</v>
       </c>
@@ -3894,7 +3828,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:5">
       <c r="A328" s="2" t="s">
         <v>330</v>
       </c>
@@ -3902,7 +3836,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:5">
       <c r="A330" s="2" t="s">
         <v>332</v>
       </c>
@@ -3910,86 +3844,86 @@
         <v>333</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:5">
       <c r="A332" s="2" t="s">
         <v>334</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="334" spans="1:2">
+      <c r="C332" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D332" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="E332" s="2"/>
+    </row>
+    <row r="334" spans="1:5">
       <c r="A334" s="2" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5">
       <c r="A336" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="338" spans="1:5">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
       <c r="A338" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="340" spans="1:5">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
       <c r="A340" s="2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="342" spans="1:5">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
       <c r="A342" s="2" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="344" spans="1:5">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
       <c r="A344" s="2" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="346" spans="1:5">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
       <c r="A346" s="2" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="348" spans="1:5">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
       <c r="A348" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C348" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D348" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E348" s="2"/>
-    </row>
-    <row r="350" spans="1:5">
+    </row>
+    <row r="350" spans="1:2">
       <c r="A350" s="2" t="s">
         <v>354</v>
       </c>
@@ -3997,7 +3931,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="352" spans="1:5">
+    <row r="352" spans="1:2">
       <c r="A352" s="2" t="s">
         <v>356</v>
       </c>
@@ -4005,7 +3939,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="354" spans="1:2">
+    <row r="354" spans="1:5">
       <c r="A354" s="2" t="s">
         <v>358</v>
       </c>
@@ -4013,7 +3947,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="356" spans="1:2">
+    <row r="356" spans="1:5">
       <c r="A356" s="2" t="s">
         <v>360</v>
       </c>
@@ -4021,7 +3955,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="358" spans="1:2">
+    <row r="358" spans="1:5">
       <c r="A358" s="2" t="s">
         <v>362</v>
       </c>
@@ -4029,7 +3963,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="360" spans="1:2">
+    <row r="360" spans="1:5">
       <c r="A360" s="2" t="s">
         <v>364</v>
       </c>
@@ -4037,7 +3971,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="362" spans="1:2">
+    <row r="362" spans="1:5">
       <c r="A362" s="2" t="s">
         <v>366</v>
       </c>
@@ -4045,7 +3979,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="364" spans="1:2">
+    <row r="364" spans="1:5">
       <c r="A364" s="2" t="s">
         <v>368</v>
       </c>
@@ -4053,1453 +3987,1373 @@
         <v>369</v>
       </c>
     </row>
-    <row r="366" spans="1:2">
+    <row r="366" spans="1:5">
       <c r="A366" s="2" t="s">
         <v>370</v>
       </c>
       <c r="B366" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5">
+      <c r="A368" s="2" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="368" spans="1:2">
-      <c r="A368" s="2" t="s">
+      <c r="B368" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B368" s="2" t="s">
+      <c r="C368" s="2"/>
+      <c r="D368" s="2"/>
+      <c r="E368" s="2"/>
+    </row>
+    <row r="370" spans="1:5">
+      <c r="A370" s="2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="370" spans="1:2">
-      <c r="A370" s="2" t="s">
+      <c r="B370" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B370" s="2" t="s">
+    </row>
+    <row r="372" spans="1:5">
+      <c r="A372" s="2" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="372" spans="1:2">
-      <c r="A372" s="2" t="s">
+      <c r="B372" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B372" s="2" t="s">
+      <c r="C372" s="2"/>
+      <c r="D372" s="2"/>
+      <c r="E372" s="2"/>
+    </row>
+    <row r="374" spans="1:5">
+      <c r="A374" s="2" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="374" spans="1:2">
-      <c r="A374" s="2" t="s">
+      <c r="B374" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B374" s="2" t="s">
+    </row>
+    <row r="376" spans="1:5">
+      <c r="A376" s="2" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="376" spans="1:2">
-      <c r="A376" s="2" t="s">
+      <c r="B376" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B376" s="2" t="s">
+    </row>
+    <row r="378" spans="1:5">
+      <c r="A378" s="2" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="378" spans="1:2">
-      <c r="A378" s="2" t="s">
+      <c r="B378" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B378" s="2" t="s">
+    </row>
+    <row r="380" spans="1:5">
+      <c r="A380" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="380" spans="1:2">
-      <c r="A380" s="2" t="s">
+      <c r="B380" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B380" s="2" t="s">
+    </row>
+    <row r="382" spans="1:5">
+      <c r="A382" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="382" spans="1:2">
-      <c r="A382" s="2" t="s">
+      <c r="B382" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B382" s="2" t="s">
+    </row>
+    <row r="384" spans="1:5">
+      <c r="A384" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="384" spans="1:2">
-      <c r="A384" s="2" t="s">
+      <c r="B384" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B384" s="2" t="s">
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" s="2" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="386" spans="1:5">
-      <c r="A386" s="2" t="s">
+      <c r="B386" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B386" s="2" t="s">
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="2" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="388" spans="1:5">
-      <c r="A388" s="2" t="s">
+      <c r="B388" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B388" s="2" t="s">
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="390" spans="1:5">
-      <c r="A390" s="2" t="s">
+      <c r="B390" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B390" s="2" t="s">
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="2" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="392" spans="1:5">
-      <c r="A392" s="2" t="s">
+      <c r="B392" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B392" s="2" t="s">
+      <c r="B394" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="394" spans="1:5">
-      <c r="A394" s="2" t="s">
+    <row r="396" spans="1:2">
+      <c r="A396" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B394" s="2" t="s">
+      <c r="B396" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="396" spans="1:5">
-      <c r="A396" s="2" t="s">
+    <row r="398" spans="1:2">
+      <c r="A398" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B396" s="2" t="s">
+      <c r="B398" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="398" spans="1:5">
-      <c r="A398" s="2" t="s">
+    <row r="400" spans="1:2">
+      <c r="A400" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B398" s="2" t="s">
+      <c r="B400" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="C398" s="2"/>
-      <c r="D398" s="2"/>
-      <c r="E398" s="2"/>
-    </row>
-    <row r="400" spans="1:5">
-      <c r="A400" s="2" t="s">
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B400" s="2" t="s">
+      <c r="B402" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="402" spans="1:5">
-      <c r="A402" s="2" t="s">
+    <row r="404" spans="1:2">
+      <c r="A404" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B402" s="2" t="s">
+      <c r="B404" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="404" spans="1:5">
-      <c r="A404" s="2" t="s">
+    <row r="406" spans="1:2">
+      <c r="A406" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B404" s="2" t="s">
+      <c r="B406" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="406" spans="1:5">
-      <c r="A406" s="2" t="s">
+    <row r="408" spans="1:2">
+      <c r="A408" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B406" s="2" t="s">
+      <c r="B408" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="C406" s="2"/>
-      <c r="D406" s="2"/>
-      <c r="E406" s="2"/>
-    </row>
-    <row r="408" spans="1:5">
-      <c r="A408" s="2" t="s">
+    </row>
+    <row r="410" spans="1:2">
+      <c r="A410" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B408" s="2" t="s">
+      <c r="B410" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="410" spans="1:5">
-      <c r="A410" s="2" t="s">
+    <row r="412" spans="1:2">
+      <c r="A412" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B410" s="2" t="s">
+      <c r="B412" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="412" spans="1:5">
-      <c r="A412" s="2" t="s">
+    <row r="414" spans="1:2">
+      <c r="A414" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B412" s="2" t="s">
+      <c r="B414" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="414" spans="1:5">
-      <c r="A414" s="2" t="s">
+    <row r="416" spans="1:2">
+      <c r="A416" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B414" s="2" t="s">
+      <c r="B416" s="2" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="416" spans="1:5">
-      <c r="A416" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="B416" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="418" spans="1:2">
       <c r="A418" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="420" spans="1:2">
       <c r="A420" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="422" spans="1:2">
       <c r="A422" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="424" spans="1:2">
       <c r="A424" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="426" spans="1:2">
       <c r="A426" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="428" spans="1:2">
       <c r="A428" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="430" spans="1:2">
       <c r="A430" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="432" spans="1:2">
       <c r="A432" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>437</v>
+        <v>238</v>
       </c>
     </row>
     <row r="434" spans="1:2">
       <c r="A434" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="436" spans="1:2">
       <c r="A436" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="438" spans="1:2">
       <c r="A438" s="2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="440" spans="1:2">
       <c r="A440" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="442" spans="1:2">
       <c r="A442" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="444" spans="1:2">
       <c r="A444" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="446" spans="1:2">
       <c r="A446" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="448" spans="1:2">
       <c r="A448" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="450" spans="1:2">
       <c r="A450" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="452" spans="1:2">
       <c r="A452" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>238</v>
+        <v>454</v>
       </c>
     </row>
     <row r="454" spans="1:2">
       <c r="A454" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="456" spans="1:2">
       <c r="A456" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="458" spans="1:2">
       <c r="A458" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="460" spans="1:2">
       <c r="A460" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="462" spans="1:2">
       <c r="A462" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="464" spans="1:2">
       <c r="A464" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="466" spans="1:2">
       <c r="A466" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="468" spans="1:2">
       <c r="A468" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="470" spans="1:2">
       <c r="A470" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="472" spans="1:2">
       <c r="A472" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="474" spans="1:2">
       <c r="A474" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="476" spans="1:2">
       <c r="A476" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="478" spans="1:2">
       <c r="A478" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="480" spans="1:2">
       <c r="A480" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="482" spans="1:2">
       <c r="A482" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="484" spans="1:2">
       <c r="A484" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="486" spans="1:2">
       <c r="A486" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="488" spans="1:2">
       <c r="A488" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="490" spans="1:2">
       <c r="A490" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="492" spans="1:2">
       <c r="A492" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="494" spans="1:2">
       <c r="A494" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="496" spans="1:2">
       <c r="A496" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="B496" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5">
+      <c r="A498" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B496" s="2" t="s">
+      <c r="B498" s="2" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="498" spans="1:2">
-      <c r="A498" s="2" t="s">
+      <c r="C498" s="2"/>
+      <c r="D498" s="2"/>
+      <c r="E498" s="2"/>
+    </row>
+    <row r="500" spans="1:5">
+      <c r="A500" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B498" s="2" t="s">
+      <c r="B500" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="500" spans="1:2">
-      <c r="A500" s="2" t="s">
+    <row r="502" spans="1:5">
+      <c r="A502" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B500" s="2" t="s">
+      <c r="B502" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="502" spans="1:2">
-      <c r="A502" s="2" t="s">
+    <row r="504" spans="1:5">
+      <c r="A504" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="B502" s="2" t="s">
+      <c r="B504" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="504" spans="1:2">
-      <c r="A504" s="2" t="s">
+    <row r="506" spans="1:5">
+      <c r="A506" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="B504" s="2" t="s">
+      <c r="B506" s="2" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="506" spans="1:2">
-      <c r="A506" s="2" t="s">
+    <row r="508" spans="1:5">
+      <c r="A508" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B506" s="2" t="s">
+      <c r="B508" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="508" spans="1:2">
-      <c r="A508" s="2" t="s">
+    <row r="510" spans="1:5">
+      <c r="A510" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="B508" s="2" t="s">
+      <c r="B510" s="2" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="510" spans="1:2">
-      <c r="A510" s="2" t="s">
+    <row r="512" spans="1:5">
+      <c r="A512" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="B510" s="2" t="s">
+      <c r="B512" s="2" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="512" spans="1:2">
-      <c r="A512" s="2" t="s">
+    <row r="514" spans="1:2">
+      <c r="A514" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="B512" s="2" t="s">
+      <c r="B514" s="2" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="514" spans="1:5">
-      <c r="A514" s="2" t="s">
+    <row r="516" spans="1:2">
+      <c r="A516" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="B514" s="2" t="s">
+      <c r="B516" s="2" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="516" spans="1:5">
-      <c r="A516" s="2" t="s">
+    <row r="518" spans="1:2">
+      <c r="A518" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B516" s="2" t="s">
+      <c r="B518" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="518" spans="1:5">
-      <c r="A518" s="2" t="s">
+    <row r="520" spans="1:2">
+      <c r="A520" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B518" s="2" t="s">
+      <c r="B520" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="C518" s="2"/>
-      <c r="D518" s="2"/>
-      <c r="E518" s="2"/>
-    </row>
-    <row r="520" spans="1:5">
-      <c r="A520" s="2" t="s">
+    </row>
+    <row r="522" spans="1:2">
+      <c r="A522" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="B520" s="2" t="s">
+      <c r="B522" s="2" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="522" spans="1:5">
-      <c r="A522" s="2" t="s">
+    <row r="524" spans="1:2">
+      <c r="A524" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B522" s="2" t="s">
+      <c r="B524" s="2" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="524" spans="1:5">
-      <c r="A524" s="2" t="s">
+    <row r="526" spans="1:2">
+      <c r="A526" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B524" s="2" t="s">
+      <c r="B526" s="2" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="526" spans="1:5">
-      <c r="A526" s="2" t="s">
+    <row r="528" spans="1:2">
+      <c r="A528" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="B526" s="2" t="s">
+      <c r="B528" s="2" t="s">
         <v>530</v>
-      </c>
-    </row>
-    <row r="528" spans="1:5">
-      <c r="A528" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="B528" s="2" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="530" spans="1:2">
       <c r="A530" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="532" spans="1:2">
       <c r="A532" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="534" spans="1:2">
       <c r="A534" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="536" spans="1:2">
       <c r="A536" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="538" spans="1:2">
       <c r="A538" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="540" spans="1:2">
       <c r="A540" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B540" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="542" spans="1:2">
       <c r="A542" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="544" spans="1:2">
       <c r="A544" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B544" s="2" t="s">
-        <v>548</v>
+        <v>415</v>
       </c>
     </row>
     <row r="546" spans="1:2">
       <c r="A546" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B546" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="548" spans="1:2">
       <c r="A548" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B548" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="550" spans="1:2">
       <c r="A550" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B550" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="552" spans="1:2">
       <c r="A552" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="554" spans="1:2">
       <c r="A554" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B554" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="556" spans="1:2">
       <c r="A556" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="558" spans="1:2">
       <c r="A558" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B558" s="2" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="560" spans="1:2">
       <c r="A560" s="2" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B560" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="562" spans="1:2">
       <c r="A562" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="564" spans="1:2">
       <c r="A564" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>435</v>
+        <v>565</v>
       </c>
     </row>
     <row r="566" spans="1:2">
       <c r="A566" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B566" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="568" spans="1:2">
       <c r="A568" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B568" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="570" spans="1:2">
       <c r="A570" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B570" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="572" spans="1:2">
       <c r="A572" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B572" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="574" spans="1:2">
       <c r="A574" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="576" spans="1:2">
       <c r="A576" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="578" spans="1:2">
       <c r="A578" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="580" spans="1:2">
       <c r="A580" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="582" spans="1:2">
       <c r="A582" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="584" spans="1:2">
       <c r="A584" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="586" spans="1:2">
       <c r="A586" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="588" spans="1:2">
       <c r="A588" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="590" spans="1:2">
       <c r="A590" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="592" spans="1:2">
       <c r="A592" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="594" spans="1:2">
       <c r="A594" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B594" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="596" spans="1:2">
       <c r="A596" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B596" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="598" spans="1:2">
       <c r="A598" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B598" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="600" spans="1:2">
       <c r="A600" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B600" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="602" spans="1:2">
       <c r="A602" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B602" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="604" spans="1:2">
       <c r="A604" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B604" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="606" spans="1:2">
       <c r="A606" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="608" spans="1:2">
       <c r="A608" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="610" spans="1:2">
       <c r="A610" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="612" spans="1:2">
       <c r="A612" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B612" s="2" t="s">
-        <v>615</v>
+        <v>577</v>
       </c>
     </row>
     <row r="614" spans="1:2">
       <c r="A614" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B614" s="2" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="616" spans="1:2">
       <c r="A616" s="2" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B616" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="618" spans="1:2">
       <c r="A618" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B618" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="620" spans="1:2">
       <c r="A620" s="2" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="622" spans="1:2">
       <c r="A622" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="624" spans="1:2">
       <c r="A624" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="626" spans="1:2">
       <c r="A626" s="2" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="628" spans="1:2">
       <c r="A628" s="2" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="630" spans="1:2">
       <c r="A630" s="2" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="632" spans="1:2">
       <c r="A632" s="2" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>599</v>
+        <v>632</v>
       </c>
     </row>
     <row r="634" spans="1:2">
       <c r="A634" s="2" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="636" spans="1:2">
       <c r="A636" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="638" spans="1:2">
       <c r="A638" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="640" spans="1:2">
       <c r="A640" s="2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="642" spans="1:2">
       <c r="A642" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="644" spans="1:2">
       <c r="A644" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="646" spans="1:2">
       <c r="A646" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="648" spans="1:2">
       <c r="A648" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="650" spans="1:2">
       <c r="A650" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="652" spans="1:2">
       <c r="A652" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="654" spans="1:2">
       <c r="A654" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="656" spans="1:2">
       <c r="A656" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="658" spans="1:2">
       <c r="A658" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="660" spans="1:2">
       <c r="A660" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="662" spans="1:2">
       <c r="A662" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="664" spans="1:2">
       <c r="A664" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="666" spans="1:2">
       <c r="A666" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="668" spans="1:2">
       <c r="A668" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="670" spans="1:2">
       <c r="A670" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="672" spans="1:2">
       <c r="A672" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="674" spans="1:2">
       <c r="A674" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B674" s="2" t="s">
-        <v>676</v>
+        <v>238</v>
       </c>
     </row>
     <row r="676" spans="1:2">
       <c r="A676" s="2" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="678" spans="1:2">
       <c r="A678" s="2" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="680" spans="1:2">
       <c r="A680" s="2" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="682" spans="1:2">
       <c r="A682" s="2" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="684" spans="1:2">
       <c r="A684" s="2" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="686" spans="1:2">
       <c r="A686" s="2" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="688" spans="1:2">
       <c r="A688" s="2" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="690" spans="1:2">
       <c r="A690" s="2" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="692" spans="1:2">
       <c r="A692" s="2" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="694" spans="1:2">
       <c r="A694" s="2" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>238</v>
+        <v>693</v>
       </c>
     </row>
     <row r="696" spans="1:2">
       <c r="A696" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>697</v>
+        <v>427</v>
       </c>
     </row>
     <row r="698" spans="1:2">
       <c r="A698" s="2" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="700" spans="1:2">
       <c r="A700" s="2" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="702" spans="1:2">
       <c r="A702" s="2" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="704" spans="1:2">
       <c r="A704" s="2" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="706" spans="1:2">
-      <c r="A706" s="2" t="s">
-        <v>706</v>
-      </c>
-      <c r="B706" s="2" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="708" spans="1:2">
-      <c r="A708" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="B708" s="2" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="710" spans="1:2">
-      <c r="A710" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="B710" s="2" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="712" spans="1:2">
-      <c r="A712" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="B712" s="2" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="714" spans="1:2">
-      <c r="A714" s="2" t="s">
-        <v>714</v>
-      </c>
-      <c r="B714" s="2" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="716" spans="1:2">
-      <c r="A716" s="2" t="s">
-        <v>716</v>
-      </c>
-      <c r="B716" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="718" spans="1:2">
-      <c r="A718" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="B718" s="2" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="720" spans="1:2">
-      <c r="A720" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="B720" s="2" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="722" spans="1:2">
-      <c r="A722" s="2" t="s">
-        <v>721</v>
-      </c>
-      <c r="B722" s="2" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="724" spans="1:2">
-      <c r="A724" s="2" t="s">
-        <v>723</v>
-      </c>
-      <c r="B724" s="2" t="s">
-        <v>724</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-01-09 16:18:13 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="701">
   <si>
     <t>Sigla</t>
   </si>
@@ -1022,12 +1022,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Mecânica Quântica</t>
-  </si>
-  <si>
-    <t>6279110</t>
-  </si>
-  <si>
-    <t>Carlos Alberto Moreira dos Santos</t>
   </si>
   <si>
     <t>LOM3227</t>
@@ -3804,7 +3798,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="322" spans="1:5">
+    <row r="322" spans="1:2">
       <c r="A322" s="2" t="s">
         <v>324</v>
       </c>
@@ -3812,7 +3806,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="324" spans="1:5">
+    <row r="324" spans="1:2">
       <c r="A324" s="2" t="s">
         <v>326</v>
       </c>
@@ -3820,7 +3814,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="326" spans="1:5">
+    <row r="326" spans="1:2">
       <c r="A326" s="2" t="s">
         <v>328</v>
       </c>
@@ -3828,7 +3822,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="328" spans="1:5">
+    <row r="328" spans="1:2">
       <c r="A328" s="2" t="s">
         <v>330</v>
       </c>
@@ -3836,7 +3830,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="330" spans="1:5">
+    <row r="330" spans="1:2">
       <c r="A330" s="2" t="s">
         <v>332</v>
       </c>
@@ -3844,152 +3838,145 @@
         <v>333</v>
       </c>
     </row>
-    <row r="332" spans="1:5">
+    <row r="332" spans="1:2">
       <c r="A332" s="2" t="s">
         <v>334</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C332" s="2" t="s">
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D332" s="2" t="s">
+      <c r="B334" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="E332" s="2"/>
-    </row>
-    <row r="334" spans="1:5">
-      <c r="A334" s="2" t="s">
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B334" s="2" t="s">
+      <c r="B336" s="2" t="s">
         <v>339</v>
-      </c>
-    </row>
-    <row r="336" spans="1:5">
-      <c r="A336" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B336" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="338" spans="1:2">
       <c r="A338" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="340" spans="1:2">
       <c r="A340" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="342" spans="1:2">
       <c r="A342" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="344" spans="1:2">
       <c r="A344" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="346" spans="1:2">
       <c r="A346" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="348" spans="1:2">
       <c r="A348" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="350" spans="1:2">
       <c r="A350" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="352" spans="1:2">
       <c r="A352" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="354" spans="1:5">
       <c r="A354" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="356" spans="1:5">
       <c r="A356" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="358" spans="1:5">
       <c r="A358" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="360" spans="1:5">
       <c r="A360" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="362" spans="1:5">
       <c r="A362" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="364" spans="1:5">
       <c r="A364" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="366" spans="1:5">
       <c r="A366" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B366" s="2" t="s">
         <v>124</v>
@@ -3997,109 +3984,106 @@
     </row>
     <row r="368" spans="1:5">
       <c r="A368" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
       <c r="E368" s="2"/>
     </row>
-    <row r="370" spans="1:5">
+    <row r="370" spans="1:2">
       <c r="A370" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B370" s="2" t="s">
+      <c r="B372" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="372" spans="1:5">
-      <c r="A372" s="2" t="s">
+    <row r="374" spans="1:2">
+      <c r="A374" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B372" s="2" t="s">
+      <c r="B374" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C372" s="2"/>
-      <c r="D372" s="2"/>
-      <c r="E372" s="2"/>
-    </row>
-    <row r="374" spans="1:5">
-      <c r="A374" s="2" t="s">
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B374" s="2" t="s">
+      <c r="B376" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="376" spans="1:5">
-      <c r="A376" s="2" t="s">
+    <row r="378" spans="1:2">
+      <c r="A378" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B376" s="2" t="s">
+      <c r="B378" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="378" spans="1:5">
-      <c r="A378" s="2" t="s">
+    <row r="380" spans="1:2">
+      <c r="A380" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B378" s="2" t="s">
+      <c r="B380" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="380" spans="1:5">
-      <c r="A380" s="2" t="s">
+    <row r="382" spans="1:2">
+      <c r="A382" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B380" s="2" t="s">
+      <c r="B382" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="382" spans="1:5">
-      <c r="A382" s="2" t="s">
+    <row r="384" spans="1:2">
+      <c r="A384" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B382" s="2" t="s">
+      <c r="B384" s="2" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="384" spans="1:5">
-      <c r="A384" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="B384" s="2" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="386" spans="1:2">
       <c r="A386" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="388" spans="1:2">
       <c r="A388" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="390" spans="1:2">
       <c r="A390" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="392" spans="1:2">
       <c r="A392" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B392" s="2" t="s">
         <v>116</v>
@@ -4107,159 +4091,159 @@
     </row>
     <row r="394" spans="1:2">
       <c r="A394" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="396" spans="1:2">
       <c r="A396" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="398" spans="1:2">
       <c r="A398" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="400" spans="1:2">
       <c r="A400" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="402" spans="1:2">
       <c r="A402" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="404" spans="1:2">
       <c r="A404" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="406" spans="1:2">
       <c r="A406" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="408" spans="1:2">
       <c r="A408" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="410" spans="1:2">
       <c r="A410" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="412" spans="1:2">
       <c r="A412" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="414" spans="1:2">
       <c r="A414" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="416" spans="1:2">
       <c r="A416" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="418" spans="1:2">
       <c r="A418" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="420" spans="1:2">
       <c r="A420" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="422" spans="1:2">
       <c r="A422" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="424" spans="1:2">
       <c r="A424" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="426" spans="1:2">
       <c r="A426" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="428" spans="1:2">
       <c r="A428" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="430" spans="1:2">
       <c r="A430" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="432" spans="1:2">
       <c r="A432" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>238</v>
@@ -4267,266 +4251,266 @@
     </row>
     <row r="434" spans="1:2">
       <c r="A434" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="436" spans="1:2">
       <c r="A436" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="438" spans="1:2">
       <c r="A438" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="440" spans="1:2">
       <c r="A440" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="442" spans="1:2">
       <c r="A442" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="444" spans="1:2">
       <c r="A444" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="446" spans="1:2">
       <c r="A446" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="448" spans="1:2">
       <c r="A448" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="450" spans="1:2">
       <c r="A450" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="452" spans="1:2">
       <c r="A452" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="454" spans="1:2">
       <c r="A454" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="456" spans="1:2">
       <c r="A456" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="458" spans="1:2">
       <c r="A458" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="460" spans="1:2">
       <c r="A460" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="462" spans="1:2">
       <c r="A462" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="464" spans="1:2">
       <c r="A464" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="466" spans="1:2">
       <c r="A466" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="468" spans="1:2">
       <c r="A468" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="470" spans="1:2">
       <c r="A470" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="472" spans="1:2">
       <c r="A472" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="474" spans="1:2">
       <c r="A474" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="476" spans="1:2">
       <c r="A476" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="478" spans="1:2">
       <c r="A478" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="480" spans="1:2">
       <c r="A480" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="482" spans="1:2">
       <c r="A482" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="484" spans="1:2">
       <c r="A484" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="486" spans="1:2">
       <c r="A486" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="488" spans="1:2">
       <c r="A488" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="490" spans="1:2">
       <c r="A490" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="492" spans="1:2">
       <c r="A492" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="494" spans="1:2">
       <c r="A494" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="496" spans="1:2">
       <c r="A496" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="498" spans="1:5">
       <c r="A498" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C498" s="2"/>
       <c r="D498" s="2"/>
@@ -4534,703 +4518,703 @@
     </row>
     <row r="500" spans="1:5">
       <c r="A500" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="502" spans="1:5">
       <c r="A502" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="504" spans="1:5">
       <c r="A504" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="506" spans="1:5">
       <c r="A506" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="508" spans="1:5">
       <c r="A508" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="510" spans="1:5">
       <c r="A510" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B510" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="512" spans="1:5">
       <c r="A512" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="514" spans="1:2">
       <c r="A514" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="516" spans="1:2">
       <c r="A516" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B516" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="518" spans="1:2">
       <c r="A518" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="520" spans="1:2">
       <c r="A520" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="522" spans="1:2">
       <c r="A522" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="524" spans="1:2">
       <c r="A524" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="526" spans="1:2">
       <c r="A526" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="528" spans="1:2">
       <c r="A528" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="530" spans="1:2">
       <c r="A530" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="532" spans="1:2">
       <c r="A532" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="534" spans="1:2">
       <c r="A534" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="536" spans="1:2">
       <c r="A536" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="538" spans="1:2">
       <c r="A538" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="540" spans="1:2">
       <c r="A540" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B540" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="542" spans="1:2">
       <c r="A542" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="544" spans="1:2">
       <c r="A544" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B544" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="546" spans="1:2">
       <c r="A546" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B546" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="548" spans="1:2">
       <c r="A548" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B548" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="550" spans="1:2">
       <c r="A550" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B550" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="552" spans="1:2">
       <c r="A552" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="554" spans="1:2">
       <c r="A554" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B554" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="556" spans="1:2">
       <c r="A556" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="558" spans="1:2">
       <c r="A558" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B558" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="560" spans="1:2">
       <c r="A560" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B560" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="562" spans="1:2">
       <c r="A562" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="564" spans="1:2">
       <c r="A564" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="566" spans="1:2">
       <c r="A566" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B566" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="568" spans="1:2">
       <c r="A568" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B568" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="570" spans="1:2">
       <c r="A570" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B570" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="572" spans="1:2">
       <c r="A572" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B572" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="574" spans="1:2">
       <c r="A574" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="576" spans="1:2">
       <c r="A576" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="578" spans="1:2">
       <c r="A578" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="580" spans="1:2">
       <c r="A580" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="582" spans="1:2">
       <c r="A582" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="584" spans="1:2">
       <c r="A584" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="586" spans="1:2">
       <c r="A586" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="588" spans="1:2">
       <c r="A588" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="590" spans="1:2">
       <c r="A590" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="592" spans="1:2">
       <c r="A592" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B592" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="594" spans="1:2">
       <c r="A594" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B594" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="596" spans="1:2">
       <c r="A596" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B596" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="598" spans="1:2">
       <c r="A598" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B598" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="600" spans="1:2">
       <c r="A600" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B600" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="602" spans="1:2">
       <c r="A602" s="2" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B602" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="604" spans="1:2">
       <c r="A604" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B604" s="2" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="606" spans="1:2">
       <c r="A606" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B606" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="608" spans="1:2">
       <c r="A608" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B608" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="610" spans="1:2">
       <c r="A610" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B610" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="612" spans="1:2">
       <c r="A612" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B612" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="614" spans="1:2">
       <c r="A614" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B614" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="616" spans="1:2">
       <c r="A616" s="2" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B616" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="618" spans="1:2">
       <c r="A618" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B618" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="620" spans="1:2">
       <c r="A620" s="2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B620" s="2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="622" spans="1:2">
       <c r="A622" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B622" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="624" spans="1:2">
       <c r="A624" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B624" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="626" spans="1:2">
       <c r="A626" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B626" s="2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="628" spans="1:2">
       <c r="A628" s="2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B628" s="2" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="630" spans="1:2">
       <c r="A630" s="2" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B630" s="2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="632" spans="1:2">
       <c r="A632" s="2" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B632" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="634" spans="1:2">
       <c r="A634" s="2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B634" s="2" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="636" spans="1:2">
       <c r="A636" s="2" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B636" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="638" spans="1:2">
       <c r="A638" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B638" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="640" spans="1:2">
       <c r="A640" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="642" spans="1:2">
       <c r="A642" s="2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="644" spans="1:2">
       <c r="A644" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B644" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="646" spans="1:2">
       <c r="A646" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B646" s="2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="648" spans="1:2">
       <c r="A648" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B648" s="2" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="650" spans="1:2">
       <c r="A650" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B650" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="652" spans="1:2">
       <c r="A652" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B652" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="654" spans="1:2">
       <c r="A654" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B654" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="656" spans="1:2">
       <c r="A656" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B656" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="658" spans="1:2">
       <c r="A658" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B658" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="660" spans="1:2">
       <c r="A660" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B660" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="662" spans="1:2">
       <c r="A662" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B662" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="664" spans="1:2">
       <c r="A664" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B664" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="666" spans="1:2">
       <c r="A666" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B666" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="668" spans="1:2">
       <c r="A668" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="670" spans="1:2">
       <c r="A670" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="672" spans="1:2">
       <c r="A672" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="674" spans="1:2">
       <c r="A674" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B674" s="2" t="s">
         <v>238</v>
@@ -5238,122 +5222,122 @@
     </row>
     <row r="676" spans="1:2">
       <c r="A676" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B676" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="678" spans="1:2">
       <c r="A678" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B678" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="680" spans="1:2">
       <c r="A680" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="682" spans="1:2">
       <c r="A682" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B682" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="684" spans="1:2">
       <c r="A684" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B684" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="686" spans="1:2">
       <c r="A686" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="688" spans="1:2">
       <c r="A688" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B688" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="690" spans="1:2">
       <c r="A690" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B690" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="692" spans="1:2">
       <c r="A692" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B692" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="694" spans="1:2">
       <c r="A694" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B694" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="696" spans="1:2">
       <c r="A696" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B696" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="698" spans="1:2">
       <c r="A698" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B698" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="700" spans="1:2">
       <c r="A700" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B700" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="702" spans="1:2">
       <c r="A702" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B702" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="704" spans="1:2">
       <c r="A704" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B704" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-09-18 16:08:07 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -7393,601 +7393,601 @@
         <v>638</v>
       </c>
       <c r="C570" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D570" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="E570" s="2"/>
+    </row>
+    <row r="571" spans="1:5">
+      <c r="C571" t="s">
         <v>613</v>
       </c>
-      <c r="D570" s="2" t="s">
+      <c r="D571" t="s">
         <v>614</v>
       </c>
-      <c r="E570" s="2"/>
-    </row>
-    <row r="572" spans="1:5">
-      <c r="A572" s="2" t="s">
+    </row>
+    <row r="573" spans="1:5">
+      <c r="A573" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="B572" s="2" t="s">
+      <c r="B573" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="C572" s="2" t="s">
+      <c r="C573" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="D572" s="2" t="s">
+      <c r="D573" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="E572" s="2"/>
-    </row>
-    <row r="574" spans="1:5">
-      <c r="A574" s="2" t="s">
+      <c r="E573" s="2"/>
+    </row>
+    <row r="575" spans="1:5">
+      <c r="A575" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="B574" s="2" t="s">
+      <c r="B575" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="C574" s="2" t="s">
+      <c r="C575" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D574" s="2" t="s">
+      <c r="D575" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E574" s="2"/>
-    </row>
-    <row r="575" spans="1:5">
-      <c r="C575" t="s">
-        <v>563</v>
-      </c>
-      <c r="D575" t="s">
-        <v>564</v>
-      </c>
+      <c r="E575" s="2"/>
     </row>
     <row r="576" spans="1:5">
       <c r="C576" t="s">
-        <v>627</v>
+        <v>563</v>
       </c>
       <c r="D576" t="s">
-        <v>628</v>
+        <v>564</v>
       </c>
     </row>
     <row r="577" spans="1:5">
       <c r="C577" t="s">
+        <v>627</v>
+      </c>
+      <c r="D577" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5">
+      <c r="C578" t="s">
         <v>526</v>
       </c>
-      <c r="D577" t="s">
+      <c r="D578" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="579" spans="1:5">
-      <c r="A579" s="2" t="s">
+    <row r="580" spans="1:5">
+      <c r="A580" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="B579" s="2" t="s">
+      <c r="B580" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="C579" s="2" t="s">
+      <c r="C580" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="D579" s="2" t="s">
+      <c r="D580" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="E579" s="2"/>
-    </row>
-    <row r="581" spans="1:5">
-      <c r="A581" s="2" t="s">
+      <c r="E580" s="2"/>
+    </row>
+    <row r="582" spans="1:5">
+      <c r="A582" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="B581" s="2" t="s">
+      <c r="B582" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="C581" s="2" t="s">
+      <c r="C582" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="D581" s="2" t="s">
+      <c r="D582" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="E581" s="2"/>
-    </row>
-    <row r="583" spans="1:5">
-      <c r="A583" s="2" t="s">
+      <c r="E582" s="2"/>
+    </row>
+    <row r="584" spans="1:5">
+      <c r="A584" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="B583" s="2" t="s">
+      <c r="B584" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="C583" s="2" t="s">
+      <c r="C584" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="D583" s="2" t="s">
+      <c r="D584" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="E583" s="2"/>
-    </row>
-    <row r="585" spans="1:5">
-      <c r="A585" s="2" t="s">
+      <c r="E584" s="2"/>
+    </row>
+    <row r="586" spans="1:5">
+      <c r="A586" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="B585" s="2" t="s">
+      <c r="B586" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="C585" s="2" t="s">
+      <c r="C586" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="D585" s="2" t="s">
+      <c r="D586" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="E585" s="2"/>
-    </row>
-    <row r="586" spans="1:5">
-      <c r="C586" t="s">
+      <c r="E586" s="2"/>
+    </row>
+    <row r="587" spans="1:5">
+      <c r="C587" t="s">
         <v>653</v>
       </c>
-      <c r="D586" t="s">
+      <c r="D587" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="588" spans="1:5">
-      <c r="A588" s="2" t="s">
+    <row r="589" spans="1:5">
+      <c r="A589" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="B588" s="2" t="s">
+      <c r="B589" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="C588" s="2" t="s">
+      <c r="C589" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="D588" s="2" t="s">
+      <c r="D589" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="E588" s="2"/>
-    </row>
-    <row r="590" spans="1:5">
-      <c r="A590" s="2" t="s">
+      <c r="E589" s="2"/>
+    </row>
+    <row r="591" spans="1:5">
+      <c r="A591" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="B590" s="2" t="s">
+      <c r="B591" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C590" s="2" t="s">
+      <c r="C591" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D590" s="2" t="s">
+      <c r="D591" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E590" s="2"/>
-    </row>
-    <row r="591" spans="1:5">
-      <c r="C591" t="s">
+      <c r="E591" s="2"/>
+    </row>
+    <row r="592" spans="1:5">
+      <c r="C592" t="s">
         <v>659</v>
       </c>
-      <c r="D591" t="s">
+      <c r="D592" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="593" spans="1:5">
-      <c r="A593" s="2" t="s">
+    <row r="594" spans="1:5">
+      <c r="A594" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="B593" s="2" t="s">
+      <c r="B594" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="C593" s="2" t="s">
+      <c r="C594" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="D593" s="2" t="s">
+      <c r="D594" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="E593" s="2"/>
-    </row>
-    <row r="594" spans="1:5">
-      <c r="C594" t="s">
+      <c r="E594" s="2"/>
+    </row>
+    <row r="595" spans="1:5">
+      <c r="C595" t="s">
         <v>659</v>
       </c>
-      <c r="D594" t="s">
+      <c r="D595" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="596" spans="1:5">
-      <c r="A596" s="2" t="s">
+    <row r="597" spans="1:5">
+      <c r="A597" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="B596" s="2" t="s">
+      <c r="B597" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="C596" s="2" t="s">
+      <c r="C597" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="D596" s="2" t="s">
+      <c r="D597" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="E596" s="2"/>
-    </row>
-    <row r="598" spans="1:5">
-      <c r="A598" s="2" t="s">
+      <c r="E597" s="2"/>
+    </row>
+    <row r="599" spans="1:5">
+      <c r="A599" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="B598" s="2" t="s">
+      <c r="B599" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="C598" s="2" t="s">
+      <c r="C599" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D598" s="2" t="s">
+      <c r="D599" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="E598" s="2"/>
-    </row>
-    <row r="599" spans="1:5">
-      <c r="C599" t="s">
+      <c r="E599" s="2"/>
+    </row>
+    <row r="600" spans="1:5">
+      <c r="C600" t="s">
         <v>653</v>
       </c>
-      <c r="D599" t="s">
+      <c r="D600" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="601" spans="1:5">
-      <c r="A601" s="2" t="s">
+    <row r="602" spans="1:5">
+      <c r="A602" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="B601" s="2" t="s">
+      <c r="B602" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="C601" s="2" t="s">
+      <c r="C602" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="D601" s="2" t="s">
+      <c r="D602" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="E601" s="2"/>
-    </row>
-    <row r="603" spans="1:5">
-      <c r="A603" s="2" t="s">
+      <c r="E602" s="2"/>
+    </row>
+    <row r="604" spans="1:5">
+      <c r="A604" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="B603" s="2" t="s">
+      <c r="B604" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="C603" s="2" t="s">
+      <c r="C604" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="D603" s="2" t="s">
+      <c r="D604" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="E603" s="2"/>
-    </row>
-    <row r="605" spans="1:5">
-      <c r="A605" s="2" t="s">
+      <c r="E604" s="2"/>
+    </row>
+    <row r="606" spans="1:5">
+      <c r="A606" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="B605" s="2" t="s">
+      <c r="B606" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="C605" s="2" t="s">
+      <c r="C606" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="D605" s="2" t="s">
+      <c r="D606" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="E605" s="2"/>
-    </row>
-    <row r="607" spans="1:5">
-      <c r="A607" s="2" t="s">
+      <c r="E606" s="2"/>
+    </row>
+    <row r="608" spans="1:5">
+      <c r="A608" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="B607" s="2" t="s">
+      <c r="B608" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="C607" s="2" t="s">
+      <c r="C608" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="D607" s="2" t="s">
+      <c r="D608" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="E607" s="2"/>
-    </row>
-    <row r="609" spans="1:5">
-      <c r="A609" s="2" t="s">
+      <c r="E608" s="2"/>
+    </row>
+    <row r="610" spans="1:5">
+      <c r="A610" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="B609" s="2" t="s">
+      <c r="B610" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="C609" s="2" t="s">
+      <c r="C610" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="D609" s="2" t="s">
+      <c r="D610" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="E609" s="2"/>
-    </row>
-    <row r="611" spans="1:5">
-      <c r="A611" s="2" t="s">
+      <c r="E610" s="2"/>
+    </row>
+    <row r="612" spans="1:5">
+      <c r="A612" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="B611" s="2" t="s">
+      <c r="B612" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="C611" s="2" t="s">
+      <c r="C612" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="D611" s="2" t="s">
+      <c r="D612" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="E611" s="2"/>
-    </row>
-    <row r="613" spans="1:5">
-      <c r="A613" s="2" t="s">
+      <c r="E612" s="2"/>
+    </row>
+    <row r="614" spans="1:5">
+      <c r="A614" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="B613" s="2" t="s">
+      <c r="B614" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="C613" s="2" t="s">
+      <c r="C614" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="D613" s="2" t="s">
+      <c r="D614" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="E613" s="2"/>
-    </row>
-    <row r="615" spans="1:5">
-      <c r="A615" s="2" t="s">
+      <c r="E614" s="2"/>
+    </row>
+    <row r="616" spans="1:5">
+      <c r="A616" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="B615" s="2" t="s">
+      <c r="B616" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="C615" s="2" t="s">
+      <c r="C616" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="D615" s="2" t="s">
+      <c r="D616" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="E615" s="2"/>
-    </row>
-    <row r="617" spans="1:5">
-      <c r="A617" s="2" t="s">
+      <c r="E616" s="2"/>
+    </row>
+    <row r="618" spans="1:5">
+      <c r="A618" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="B617" s="2" t="s">
+      <c r="B618" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="C617" s="2" t="s">
+      <c r="C618" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="D617" s="2" t="s">
+      <c r="D618" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="E617" s="2"/>
-    </row>
-    <row r="619" spans="1:5">
-      <c r="A619" s="2" t="s">
+      <c r="E618" s="2"/>
+    </row>
+    <row r="620" spans="1:5">
+      <c r="A620" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="B619" s="2" t="s">
+      <c r="B620" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="C619" s="2" t="s">
+      <c r="C620" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D619" s="2" t="s">
+      <c r="D620" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E619" s="2"/>
-    </row>
-    <row r="621" spans="1:5">
-      <c r="A621" s="2" t="s">
+      <c r="E620" s="2"/>
+    </row>
+    <row r="622" spans="1:5">
+      <c r="A622" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="B621" s="2" t="s">
+      <c r="B622" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="C621" s="2" t="s">
+      <c r="C622" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="D621" s="2" t="s">
+      <c r="D622" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="E621" s="2"/>
-    </row>
-    <row r="623" spans="1:5">
-      <c r="A623" s="2" t="s">
+      <c r="E622" s="2"/>
+    </row>
+    <row r="624" spans="1:5">
+      <c r="A624" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="B623" s="2" t="s">
+      <c r="B624" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="C623" s="2" t="s">
+      <c r="C624" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="D623" s="2" t="s">
+      <c r="D624" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="E623" s="2"/>
-    </row>
-    <row r="625" spans="1:5">
-      <c r="A625" s="2" t="s">
+      <c r="E624" s="2"/>
+    </row>
+    <row r="626" spans="1:5">
+      <c r="A626" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="B625" s="2" t="s">
+      <c r="B626" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="C625" s="2" t="s">
+      <c r="C626" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="D625" s="2" t="s">
+      <c r="D626" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="E625" s="2"/>
-    </row>
-    <row r="627" spans="1:5">
-      <c r="A627" s="2" t="s">
+      <c r="E626" s="2"/>
+    </row>
+    <row r="628" spans="1:5">
+      <c r="A628" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="B627" s="2" t="s">
+      <c r="B628" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="C627" s="2" t="s">
+      <c r="C628" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="D627" s="2" t="s">
+      <c r="D628" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="E627" s="2"/>
-    </row>
-    <row r="629" spans="1:5">
-      <c r="A629" s="2" t="s">
+      <c r="E628" s="2"/>
+    </row>
+    <row r="630" spans="1:5">
+      <c r="A630" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="B629" s="2" t="s">
+      <c r="B630" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="C629" s="2" t="s">
+      <c r="C630" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D629" s="2" t="s">
+      <c r="D630" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E629" s="2"/>
-    </row>
-    <row r="631" spans="1:5">
-      <c r="A631" s="2" t="s">
+      <c r="E630" s="2"/>
+    </row>
+    <row r="632" spans="1:5">
+      <c r="A632" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="B631" s="2" t="s">
+      <c r="B632" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="C631" s="2" t="s">
+      <c r="C632" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D631" s="2" t="s">
+      <c r="D632" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E631" s="2"/>
-    </row>
-    <row r="633" spans="1:5">
-      <c r="A633" s="2" t="s">
+      <c r="E632" s="2"/>
+    </row>
+    <row r="634" spans="1:5">
+      <c r="A634" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="B633" s="2" t="s">
+      <c r="B634" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="C633" s="2" t="s">
+      <c r="C634" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D633" s="2" t="s">
+      <c r="D634" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E633" s="2"/>
-    </row>
-    <row r="635" spans="1:5">
-      <c r="A635" s="2" t="s">
+      <c r="E634" s="2"/>
+    </row>
+    <row r="636" spans="1:5">
+      <c r="A636" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="B635" s="2" t="s">
+      <c r="B636" s="2" t="s">
         <v>708</v>
       </c>
-      <c r="C635" s="2" t="s">
+      <c r="C636" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D635" s="2" t="s">
+      <c r="D636" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E635" s="2"/>
-    </row>
-    <row r="637" spans="1:5">
-      <c r="A637" s="2" t="s">
+      <c r="E636" s="2"/>
+    </row>
+    <row r="638" spans="1:5">
+      <c r="A638" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="B637" s="2" t="s">
+      <c r="B638" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="C637" s="2" t="s">
+      <c r="C638" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D637" s="2" t="s">
+      <c r="D638" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E637" s="2"/>
-    </row>
-    <row r="639" spans="1:5">
-      <c r="A639" s="2" t="s">
+      <c r="E638" s="2"/>
+    </row>
+    <row r="640" spans="1:5">
+      <c r="A640" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="B639" s="2" t="s">
+      <c r="B640" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="C639" s="2" t="s">
+      <c r="C640" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D639" s="2" t="s">
+      <c r="D640" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E639" s="2"/>
-    </row>
-    <row r="641" spans="1:5">
-      <c r="A641" s="2" t="s">
+      <c r="E640" s="2"/>
+    </row>
+    <row r="642" spans="1:5">
+      <c r="A642" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="B641" s="2" t="s">
+      <c r="B642" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="C641" s="2" t="s">
+      <c r="C642" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D641" s="2" t="s">
+      <c r="D642" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E641" s="2"/>
-    </row>
-    <row r="643" spans="1:5">
-      <c r="A643" s="2" t="s">
+      <c r="E642" s="2"/>
+    </row>
+    <row r="644" spans="1:5">
+      <c r="A644" s="2" t="s">
         <v>715</v>
       </c>
-      <c r="B643" s="2" t="s">
+      <c r="B644" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="C643" s="2" t="s">
+      <c r="C644" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D643" s="2" t="s">
+      <c r="D644" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E643" s="2"/>
-    </row>
-    <row r="645" spans="1:5">
-      <c r="A645" s="2" t="s">
+      <c r="E644" s="2"/>
+    </row>
+    <row r="646" spans="1:5">
+      <c r="A646" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="B645" s="2" t="s">
+      <c r="B646" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="C645" s="2" t="s">
+      <c r="C646" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D645" s="2" t="s">
+      <c r="D646" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E645" s="2"/>
-    </row>
-    <row r="647" spans="1:5">
-      <c r="A647" s="2" t="s">
+      <c r="E646" s="2"/>
+    </row>
+    <row r="648" spans="1:5">
+      <c r="A648" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="B647" s="2" t="s">
+      <c r="B648" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="C647" s="2" t="s">
+      <c r="C648" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="D647" s="2" t="s">
+      <c r="D648" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="E647" s="2"/>
-    </row>
-    <row r="648" spans="1:5">
-      <c r="C648" t="s">
-        <v>559</v>
-      </c>
-      <c r="D648" t="s">
-        <v>560</v>
-      </c>
+      <c r="E648" s="2"/>
     </row>
     <row r="650" spans="1:5">
       <c r="A650" s="2" t="s">

</xml_diff>

<commit_message>
Build site at 2024-05-20 14:07:48 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="906">
   <si>
     <t>Sigla</t>
   </si>
@@ -2452,12 +2452,6 @@
     <t>Maria Eleonora Andrade de Carvalho</t>
   </si>
   <si>
-    <t>LOT2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Engenharia Ambiental</t>
-  </si>
-  <si>
     <t>LOT2013</t>
   </si>
   <si>
@@ -2726,6 +2720,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Tecnologia de Biopolímeros</t>
+  </si>
+  <si>
+    <t>LOT2061</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Química Analítica Aplicada a Bioprocessos</t>
+  </si>
+  <si>
+    <t>LOT2062</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Solução de Problemas de Engenharia</t>
   </si>
 </sst>
 </file>
@@ -3076,7 +3082,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E813"/>
+  <dimension ref="A1:E815"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8678,55 +8684,55 @@
         <v>813</v>
       </c>
       <c r="C736" s="2" t="s">
-        <v>231</v>
+        <v>814</v>
       </c>
       <c r="D736" s="2" t="s">
-        <v>232</v>
+        <v>815</v>
       </c>
       <c r="E736" s="2"/>
     </row>
     <row r="738" spans="1:5">
       <c r="A738" s="2" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B738" s="2" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C738" s="2" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="D738" s="2" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="E738" s="2"/>
     </row>
     <row r="740" spans="1:5">
       <c r="A740" s="2" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B740" s="2" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="C740" s="2" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D740" s="2" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="E740" s="2"/>
     </row>
     <row r="742" spans="1:5">
       <c r="A742" s="2" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B742" s="2" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C742" s="2" t="s">
-        <v>824</v>
+        <v>804</v>
       </c>
       <c r="D742" s="2" t="s">
-        <v>825</v>
+        <v>805</v>
       </c>
       <c r="E742" s="2"/>
     </row>
@@ -8738,55 +8744,55 @@
         <v>827</v>
       </c>
       <c r="C744" s="2" t="s">
-        <v>804</v>
+        <v>828</v>
       </c>
       <c r="D744" s="2" t="s">
-        <v>805</v>
+        <v>829</v>
       </c>
       <c r="E744" s="2"/>
     </row>
     <row r="746" spans="1:5">
       <c r="A746" s="2" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B746" s="2" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="C746" s="2" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="D746" s="2" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="E746" s="2"/>
     </row>
     <row r="748" spans="1:5">
       <c r="A748" s="2" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B748" s="2" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C748" s="2" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D748" s="2" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="E748" s="2"/>
     </row>
     <row r="750" spans="1:5">
       <c r="A750" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="B750" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="C750" s="2" t="s">
         <v>836</v>
       </c>
-      <c r="B750" s="2" t="s">
+      <c r="D750" s="2" t="s">
         <v>837</v>
-      </c>
-      <c r="C750" s="2" t="s">
-        <v>838</v>
-      </c>
-      <c r="D750" s="2" t="s">
-        <v>839</v>
       </c>
       <c r="E750" s="2"/>
     </row>
@@ -8798,25 +8804,25 @@
         <v>841</v>
       </c>
       <c r="C752" s="2" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="D752" s="2" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="E752" s="2"/>
     </row>
     <row r="754" spans="1:5">
       <c r="A754" s="2" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B754" s="2" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="C754" s="2" t="s">
-        <v>844</v>
+        <v>231</v>
       </c>
       <c r="D754" s="2" t="s">
-        <v>845</v>
+        <v>232</v>
       </c>
       <c r="E754" s="2"/>
     </row>
@@ -8828,10 +8834,10 @@
         <v>847</v>
       </c>
       <c r="C756" s="2" t="s">
-        <v>231</v>
+        <v>842</v>
       </c>
       <c r="D756" s="2" t="s">
-        <v>232</v>
+        <v>843</v>
       </c>
       <c r="E756" s="2"/>
     </row>
@@ -8843,63 +8849,63 @@
         <v>849</v>
       </c>
       <c r="C758" s="2" t="s">
-        <v>844</v>
+        <v>818</v>
       </c>
       <c r="D758" s="2" t="s">
-        <v>845</v>
+        <v>819</v>
       </c>
       <c r="E758" s="2"/>
     </row>
-    <row r="760" spans="1:5">
-      <c r="A760" s="2" t="s">
+    <row r="759" spans="1:5">
+      <c r="C759" t="s">
         <v>850</v>
       </c>
-      <c r="B760" s="2" t="s">
+      <c r="D759" t="s">
         <v>851</v>
       </c>
-      <c r="C760" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="D760" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="E760" s="2"/>
     </row>
     <row r="761" spans="1:5">
-      <c r="C761" t="s">
+      <c r="A761" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="D761" t="s">
+      <c r="B761" s="2" t="s">
         <v>853</v>
       </c>
+      <c r="C761" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="D761" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="E761" s="2"/>
     </row>
     <row r="763" spans="1:5">
       <c r="A763" s="2" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B763" s="2" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C763" s="2" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D763" s="2" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="E763" s="2"/>
     </row>
     <row r="765" spans="1:5">
       <c r="A765" s="2" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="B765" s="2" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C765" s="2" t="s">
-        <v>860</v>
+        <v>794</v>
       </c>
       <c r="D765" s="2" t="s">
-        <v>861</v>
+        <v>795</v>
       </c>
       <c r="E765" s="2"/>
     </row>
@@ -8911,35 +8917,35 @@
         <v>863</v>
       </c>
       <c r="C767" s="2" t="s">
-        <v>794</v>
+        <v>832</v>
       </c>
       <c r="D767" s="2" t="s">
-        <v>795</v>
+        <v>833</v>
       </c>
       <c r="E767" s="2"/>
     </row>
-    <row r="769" spans="1:5">
-      <c r="A769" s="2" t="s">
+    <row r="768" spans="1:5">
+      <c r="C768" t="s">
+        <v>854</v>
+      </c>
+      <c r="D768" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="770" spans="1:5">
+      <c r="A770" s="2" t="s">
         <v>864</v>
       </c>
-      <c r="B769" s="2" t="s">
+      <c r="B770" s="2" t="s">
         <v>865</v>
       </c>
-      <c r="C769" s="2" t="s">
-        <v>834</v>
-      </c>
-      <c r="D769" s="2" t="s">
-        <v>835</v>
-      </c>
-      <c r="E769" s="2"/>
-    </row>
-    <row r="770" spans="1:5">
-      <c r="C770" t="s">
-        <v>856</v>
-      </c>
-      <c r="D770" t="s">
-        <v>857</v>
-      </c>
+      <c r="C770" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="D770" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="E770" s="2"/>
     </row>
     <row r="772" spans="1:5">
       <c r="A772" s="2" t="s">
@@ -8949,48 +8955,48 @@
         <v>867</v>
       </c>
       <c r="C772" s="2" t="s">
-        <v>830</v>
+        <v>818</v>
       </c>
       <c r="D772" s="2" t="s">
-        <v>831</v>
+        <v>819</v>
       </c>
       <c r="E772" s="2"/>
     </row>
-    <row r="774" spans="1:5">
-      <c r="A774" s="2" t="s">
+    <row r="773" spans="1:5">
+      <c r="C773" t="s">
         <v>868</v>
       </c>
-      <c r="B774" s="2" t="s">
+      <c r="D773" t="s">
         <v>869</v>
       </c>
-      <c r="C774" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="D774" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="E774" s="2"/>
     </row>
     <row r="775" spans="1:5">
-      <c r="C775" t="s">
+      <c r="A775" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="D775" t="s">
-        <v>871</v>
-      </c>
+      <c r="B775" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C775" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="D775" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="E775" s="2"/>
     </row>
     <row r="777" spans="1:5">
       <c r="A777" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B777" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="B777" s="2" t="s">
-        <v>342</v>
-      </c>
       <c r="C777" s="2" t="s">
-        <v>820</v>
+        <v>788</v>
       </c>
       <c r="D777" s="2" t="s">
-        <v>821</v>
+        <v>789</v>
       </c>
       <c r="E777" s="2"/>
     </row>
@@ -9017,10 +9023,10 @@
         <v>876</v>
       </c>
       <c r="C781" s="2" t="s">
-        <v>788</v>
+        <v>850</v>
       </c>
       <c r="D781" s="2" t="s">
-        <v>789</v>
+        <v>851</v>
       </c>
       <c r="E781" s="2"/>
     </row>
@@ -9032,10 +9038,10 @@
         <v>878</v>
       </c>
       <c r="C783" s="2" t="s">
-        <v>852</v>
+        <v>794</v>
       </c>
       <c r="D783" s="2" t="s">
-        <v>853</v>
+        <v>795</v>
       </c>
       <c r="E783" s="2"/>
     </row>
@@ -9047,35 +9053,35 @@
         <v>880</v>
       </c>
       <c r="C785" s="2" t="s">
-        <v>794</v>
+        <v>881</v>
       </c>
       <c r="D785" s="2" t="s">
-        <v>795</v>
+        <v>882</v>
       </c>
       <c r="E785" s="2"/>
     </row>
-    <row r="787" spans="1:5">
-      <c r="A787" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="B787" s="2" t="s">
-        <v>882</v>
-      </c>
-      <c r="C787" s="2" t="s">
+    <row r="786" spans="1:5">
+      <c r="C786" t="s">
+        <v>790</v>
+      </c>
+      <c r="D786" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="788" spans="1:5">
+      <c r="A788" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="D787" s="2" t="s">
+      <c r="B788" s="2" t="s">
         <v>884</v>
       </c>
-      <c r="E787" s="2"/>
-    </row>
-    <row r="788" spans="1:5">
-      <c r="C788" t="s">
-        <v>790</v>
-      </c>
-      <c r="D788" t="s">
-        <v>791</v>
-      </c>
+      <c r="C788" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="D788" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="E788" s="2"/>
     </row>
     <row r="790" spans="1:5">
       <c r="A790" s="2" t="s">
@@ -9085,10 +9091,10 @@
         <v>886</v>
       </c>
       <c r="C790" s="2" t="s">
-        <v>820</v>
+        <v>854</v>
       </c>
       <c r="D790" s="2" t="s">
-        <v>821</v>
+        <v>855</v>
       </c>
       <c r="E790" s="2"/>
     </row>
@@ -9100,35 +9106,35 @@
         <v>888</v>
       </c>
       <c r="C792" s="2" t="s">
-        <v>856</v>
+        <v>822</v>
       </c>
       <c r="D792" s="2" t="s">
-        <v>857</v>
+        <v>823</v>
       </c>
       <c r="E792" s="2"/>
     </row>
-    <row r="794" spans="1:5">
-      <c r="A794" s="2" t="s">
+    <row r="793" spans="1:5">
+      <c r="C793" t="s">
+        <v>881</v>
+      </c>
+      <c r="D793" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="795" spans="1:5">
+      <c r="A795" s="2" t="s">
         <v>889</v>
       </c>
-      <c r="B794" s="2" t="s">
+      <c r="B795" s="2" t="s">
         <v>890</v>
       </c>
-      <c r="C794" s="2" t="s">
-        <v>824</v>
-      </c>
-      <c r="D794" s="2" t="s">
-        <v>825</v>
-      </c>
-      <c r="E794" s="2"/>
-    </row>
-    <row r="795" spans="1:5">
-      <c r="C795" t="s">
-        <v>883</v>
-      </c>
-      <c r="D795" t="s">
-        <v>884</v>
-      </c>
+      <c r="C795" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="D795" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="E795" s="2"/>
     </row>
     <row r="797" spans="1:5">
       <c r="A797" s="2" t="s">
@@ -9138,10 +9144,10 @@
         <v>892</v>
       </c>
       <c r="C797" s="2" t="s">
-        <v>790</v>
+        <v>868</v>
       </c>
       <c r="D797" s="2" t="s">
-        <v>791</v>
+        <v>869</v>
       </c>
       <c r="E797" s="2"/>
     </row>
@@ -9150,107 +9156,107 @@
         <v>893</v>
       </c>
       <c r="B799" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C799" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="D799" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="E799" s="2"/>
+    </row>
+    <row r="800" spans="1:5">
+      <c r="C800" t="s">
+        <v>790</v>
+      </c>
+      <c r="D800" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="802" spans="1:5">
+      <c r="A802" s="2" t="s">
         <v>894</v>
       </c>
-      <c r="C799" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="D799" s="2" t="s">
-        <v>871</v>
-      </c>
-      <c r="E799" s="2"/>
-    </row>
-    <row r="801" spans="1:5">
-      <c r="A801" s="2" t="s">
+      <c r="B802" s="2" t="s">
         <v>895</v>
       </c>
-      <c r="B801" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C801" s="2" t="s">
+      <c r="C802" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="D801" s="2" t="s">
+      <c r="D802" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="E801" s="2"/>
-    </row>
-    <row r="802" spans="1:5">
-      <c r="C802" t="s">
+      <c r="E802" s="2"/>
+    </row>
+    <row r="803" spans="1:5">
+      <c r="C803" t="s">
         <v>790</v>
       </c>
-      <c r="D802" t="s">
+      <c r="D803" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="804" spans="1:5">
-      <c r="A804" s="2" t="s">
+    <row r="805" spans="1:5">
+      <c r="A805" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="B804" s="2" t="s">
+      <c r="B805" s="2" t="s">
         <v>897</v>
       </c>
-      <c r="C804" s="2" t="s">
-        <v>788</v>
-      </c>
-      <c r="D804" s="2" t="s">
-        <v>789</v>
-      </c>
-      <c r="E804" s="2"/>
-    </row>
-    <row r="805" spans="1:5">
-      <c r="C805" t="s">
-        <v>790</v>
-      </c>
-      <c r="D805" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="807" spans="1:5">
-      <c r="A807" s="2" t="s">
+      <c r="C805" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="D805" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="E805" s="2"/>
+    </row>
+    <row r="806" spans="1:5">
+      <c r="C806" t="s">
+        <v>868</v>
+      </c>
+      <c r="D806" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="808" spans="1:5">
+      <c r="A808" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="B807" s="2" t="s">
+      <c r="B808" s="2" t="s">
         <v>899</v>
       </c>
-      <c r="C807" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="D807" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="E807" s="2"/>
-    </row>
-    <row r="808" spans="1:5">
-      <c r="C808" t="s">
-        <v>870</v>
-      </c>
-      <c r="D808" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="810" spans="1:5">
-      <c r="A810" s="2" t="s">
+      <c r="C808" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D808" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="E808" s="2"/>
+    </row>
+    <row r="809" spans="1:5">
+      <c r="C809" t="s">
+        <v>858</v>
+      </c>
+      <c r="D809" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="811" spans="1:5">
+      <c r="A811" s="2" t="s">
         <v>900</v>
       </c>
-      <c r="B810" s="2" t="s">
+      <c r="B811" s="2" t="s">
         <v>901</v>
       </c>
-      <c r="C810" s="2" t="s">
-        <v>844</v>
-      </c>
-      <c r="D810" s="2" t="s">
-        <v>845</v>
-      </c>
-      <c r="E810" s="2"/>
-    </row>
-    <row r="811" spans="1:5">
-      <c r="C811" t="s">
-        <v>860</v>
-      </c>
-      <c r="D811" t="s">
-        <v>861</v>
-      </c>
+      <c r="C811" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="D811" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="E811" s="2"/>
     </row>
     <row r="813" spans="1:5">
       <c r="A813" s="2" t="s">
@@ -9259,13 +9265,20 @@
       <c r="B813" s="2" t="s">
         <v>903</v>
       </c>
-      <c r="C813" s="2" t="s">
-        <v>796</v>
-      </c>
-      <c r="D813" s="2" t="s">
-        <v>797</v>
-      </c>
+      <c r="C813" s="2"/>
+      <c r="D813" s="2"/>
       <c r="E813" s="2"/>
+    </row>
+    <row r="815" spans="1:5">
+      <c r="A815" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B815" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="C815" s="2"/>
+      <c r="D815" s="2"/>
+      <c r="E815" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Build site at 2024-07-31 18:20:16 UTC
</commit_message>
<xml_diff>
--- a/_python/docentes-responsaveis.xlsx
+++ b/_python/docentes-responsaveis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="904">
   <si>
     <t>Sigla</t>
   </si>
@@ -2588,12 +2588,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Tecnologia de Bebidas</t>
-  </si>
-  <si>
-    <t>1097178</t>
-  </si>
-  <si>
-    <t>João Batista de Almeida e Silva</t>
   </si>
   <si>
     <t>LOT2039</t>
@@ -3082,7 +3076,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E842"/>
+  <dimension ref="A1:E848"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8999,20 +8993,16 @@
       <c r="B778" s="2" t="s">
         <v>857</v>
       </c>
-      <c r="C778" s="2" t="s">
-        <v>858</v>
-      </c>
-      <c r="D778" s="2" t="s">
-        <v>859</v>
-      </c>
+      <c r="C778" s="2"/>
+      <c r="D778" s="2"/>
       <c r="E778" s="2"/>
     </row>
     <row r="780" spans="1:5">
       <c r="A780" s="2" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C780" s="2" t="s">
         <v>842</v>
@@ -9024,18 +9014,18 @@
     </row>
     <row r="781" spans="1:5">
       <c r="C781" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D781" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="783" spans="1:5">
       <c r="A783" s="2" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C783" s="2" t="s">
         <v>794</v>
@@ -9055,10 +9045,10 @@
     </row>
     <row r="786" spans="1:5">
       <c r="A786" s="2" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C786" s="2" t="s">
         <v>812</v>
@@ -9078,10 +9068,10 @@
     </row>
     <row r="789" spans="1:5">
       <c r="A789" s="2" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C789" s="2" t="s">
         <v>800</v>
@@ -9101,10 +9091,10 @@
     </row>
     <row r="792" spans="1:5">
       <c r="A792" s="2" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C792" s="2" t="s">
         <v>818</v>
@@ -9124,7 +9114,7 @@
     </row>
     <row r="795" spans="1:5">
       <c r="A795" s="2" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B795" s="2" t="s">
         <v>340</v>
@@ -9139,10 +9129,10 @@
     </row>
     <row r="797" spans="1:5">
       <c r="A797" s="2" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C797" s="2" t="s">
         <v>786</v>
@@ -9154,10 +9144,10 @@
     </row>
     <row r="799" spans="1:5">
       <c r="A799" s="2" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C799" s="2" t="s">
         <v>786</v>
@@ -9177,10 +9167,10 @@
     </row>
     <row r="802" spans="1:5">
       <c r="A802" s="2" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C802" s="2" t="s">
         <v>798</v>
@@ -9216,10 +9206,10 @@
     </row>
     <row r="807" spans="1:5">
       <c r="A807" s="2" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B807" s="2" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C807" s="2" t="s">
         <v>794</v>
@@ -9239,10 +9229,10 @@
     </row>
     <row r="810" spans="1:5">
       <c r="A810" s="2" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C810" s="2" t="s">
         <v>786</v>
@@ -9262,10 +9252,10 @@
     </row>
     <row r="813" spans="1:5">
       <c r="A813" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C813" s="2" t="s">
         <v>818</v>
@@ -9277,25 +9267,21 @@
     </row>
     <row r="815" spans="1:5">
       <c r="A815" s="2" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>886</v>
-      </c>
-      <c r="C815" s="2" t="s">
-        <v>858</v>
-      </c>
-      <c r="D815" s="2" t="s">
-        <v>859</v>
-      </c>
+        <v>884</v>
+      </c>
+      <c r="C815" s="2"/>
+      <c r="D815" s="2"/>
       <c r="E815" s="2"/>
     </row>
     <row r="817" spans="1:5">
       <c r="A817" s="2" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C817" s="2" t="s">
         <v>824</v>
@@ -9315,10 +9301,10 @@
     </row>
     <row r="820" spans="1:5">
       <c r="A820" s="2" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C820" s="2" t="s">
         <v>794</v>
@@ -9338,10 +9324,10 @@
     </row>
     <row r="823" spans="1:5">
       <c r="A823" s="2" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C823" s="2" t="s">
         <v>828</v>
@@ -9353,7 +9339,7 @@
     </row>
     <row r="825" spans="1:5">
       <c r="A825" s="2" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B825" s="2" t="s">
         <v>549</v>
@@ -9376,10 +9362,10 @@
     </row>
     <row r="828" spans="1:5">
       <c r="A828" s="2" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="C828" s="2" t="s">
         <v>786</v>
@@ -9399,10 +9385,10 @@
     </row>
     <row r="831" spans="1:5">
       <c r="A831" s="2" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C831" s="2" t="s">
         <v>854</v>
@@ -9422,16 +9408,16 @@
     </row>
     <row r="834" spans="1:5">
       <c r="A834" s="2" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C834" s="2" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D834" s="2" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E834" s="2"/>
     </row>
@@ -9445,10 +9431,10 @@
     </row>
     <row r="837" spans="1:5">
       <c r="A837" s="2" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C837" s="2" t="s">
         <v>844</v>
@@ -9468,29 +9454,81 @@
     </row>
     <row r="840" spans="1:5">
       <c r="A840" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B840" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="C840" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D840" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="E840" s="2"/>
+    </row>
+    <row r="841" spans="1:5">
+      <c r="C841" t="s">
+        <v>844</v>
+      </c>
+      <c r="D841" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="843" spans="1:5">
+      <c r="A843" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="B840" s="2" t="s">
+      <c r="B843" s="2" t="s">
         <v>903</v>
       </c>
-      <c r="C840" s="2"/>
-      <c r="D840" s="2"/>
-      <c r="E840" s="2"/>
-    </row>
-    <row r="842" spans="1:5">
-      <c r="A842" s="2" t="s">
-        <v>904</v>
-      </c>
-      <c r="B842" s="2" t="s">
-        <v>905</v>
-      </c>
-      <c r="C842" s="2" t="s">
+      <c r="C843" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D843" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="E843" s="2"/>
+    </row>
+    <row r="844" spans="1:5">
+      <c r="C844" t="s">
+        <v>800</v>
+      </c>
+      <c r="D844" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="845" spans="1:5">
+      <c r="C845" t="s">
+        <v>824</v>
+      </c>
+      <c r="D845" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="846" spans="1:5">
+      <c r="C846" t="s">
+        <v>804</v>
+      </c>
+      <c r="D846" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="847" spans="1:5">
+      <c r="C847" t="s">
         <v>844</v>
       </c>
-      <c r="D842" s="2" t="s">
+      <c r="D847" t="s">
         <v>845</v>
       </c>
-      <c r="E842" s="2"/>
+    </row>
+    <row r="848" spans="1:5">
+      <c r="C848" t="s">
+        <v>828</v>
+      </c>
+      <c r="D848" t="s">
+        <v>829</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>